<commit_message>
Create semantic search PoC version
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -543,7 +543,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>['resistance of materials', 'energy audit', 'building performance']</t>
+          <t>['resistance of materials', 'EU energy label', 'project funding', 'clean technology', 'cultural heritage', 'EU initiative', 'energy savings', 'seismic engineering', 'advanced materials', 'building renovation']</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
@@ -590,7 +590,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>['smart city', 'Internet of Things', 'smart technology', 'prospective technological studies', 'smart specialisation']</t>
+          <t>['smart city', 'smart technology', 'smart specialisation', 'open science', 'popularising science', 'knowledge economy', 'bibliometric analysis', 'scientific publications', 'technological innovation', 'concentration of the population']</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -641,7 +641,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>['adaptation to climate change', 'climate security', 'natural disaster', 'crisis management', 'geographical information system']</t>
+          <t>['adaptation to climate change', 'services of general interest', 'impact of information technology', 'search and rescue', 'crisis management', 'knowledge management', 'carbon capture and storage', 'Paris Agreement on Climate Change', 'risk management', 'economic instrument for the environment']</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
@@ -698,7 +698,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>['adaptation to climate change', 'community resilience', 'citizen science', 'natural disaster', 'popularising science']</t>
+          <t>['knowledge management', 'disaster prevention', 'risk assessment', 'climate change', 'risk communication', 'scientific research', 'decision-making process', 'resilience', 'transboundary cooperation', 'social dimension']</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
@@ -725,10 +725,10 @@
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="S5" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="6">
@@ -749,7 +749,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>['municipal waste', 'waste recycling', 'circular economy']</t>
+          <t>['waste recycling', 'municipal waste', 'circular economy', 'social labelling', 'pre-packaging', 'economic instrument for the environment', 'hazardous waste', 'hygiene product', 'environmental tax', 'product recall']</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
@@ -779,7 +779,7 @@
         <v>0.3333333333333333</v>
       </c>
       <c r="S6" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="7">
@@ -800,7 +800,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>['data sharing', 'European Interoperability Framework', 'systems interconnection', 'data governance']</t>
+          <t>['data sharing', 'spatial data', 'data governance', 'technical standard', 'European Interoperability Framework', 'machine-readable data', 'public data', 'open data', 'satellite data', 'technical barriers to trade']</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
@@ -851,7 +851,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>['EU study report', 'EU reference laboratory']</t>
+          <t>['aid evaluation', 'EU initiative', 'data governance', 'evaluation method', 'project evaluation', 'policy analysis', 'EU financial instrument', 'on line data service', 'multi-level governance', 'European Data Protection Board']</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
@@ -878,10 +878,10 @@
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
       <c r="R8" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="S8" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="9">
@@ -903,7 +903,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>['quality standard', 'ecodesign']</t>
+          <t>['economic instrument for the environment', 'degradation of the environment', 'quality of the environment', 'competence of the institution', 'opinion of the Commission', 'implementation of the budget', 'operation of the Institutions', 'liberalisation of the market', 'adoption of the budget', 'Institution of the Union']</t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
@@ -954,7 +954,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>['EU study report', 'EU policy - national policy', 'prospective technological studies']</t>
+          <t>['policy analysis', 'knowledge economy', 'EU study report', 'Internet of Things', 'impact of information technology', 'monitoring report', 'promotion of the European idea', 'adoption of the budget', 'liberalisation of the market', 'operation of the Institutions']</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>['supply chain', 'raw material', 'terms of trade', 'EU market']</t>
+          <t>['trade agreement (EU)', 'terms of trade', 'supply chain', 'raw material', 'value chain', 'EU strategy', 'technical barriers to trade', 'country of origin principle', 'economic governance (EU)', 'Central and Eastern European countries']</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
@@ -1035,7 +1035,7 @@
         <v>0.3333333333333333</v>
       </c>
       <c r="S11" t="n">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="12">
@@ -1056,7 +1056,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>['crop rotation', 'agricultural economics', 'precision agriculture']</t>
+          <t>['Southern neighbourhood', 'Union for the Mediterranean', 'mode of production', 'impact of information technology', 'reform of the CAP', 'economic instrument for the environment', 'sea level rise', 'concentration of the population', 'composition of the population', 'right to development']</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>['smart technology', 'European Interoperability Framework', 'systems interconnection']</t>
+          <t>['smart technology', 'liberalisation of the market', 'economic instrument for the environment', 'European Interoperability Framework', 'public policy', 'energy poverty', 'smart specialisation', 'withdrawal from the market', 'interoperability', 'consumer empowerment']</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
@@ -1134,10 +1134,10 @@
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
       <c r="R13" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="S13" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="14">
@@ -1158,7 +1158,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>['aviation security', 'critical infrastructure security', 'drone']</t>
+          <t>['critical infrastructure security', 'aviation security', 'common security and defence policy', 'public-private partnership', 'area of freedom', 'security and justice', 'systems interconnection', 'impact of information technology', 'Internet of Things', 'climate security', 'text and data mining']</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
@@ -1185,10 +1185,10 @@
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="S14" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.09090909090909091</v>
       </c>
     </row>
     <row r="15">
@@ -1209,7 +1209,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>['digital transformation', 'impact of information technology', 'economic intelligence', 'economic governance (EU)']</t>
+          <t>['digital transformation', 'digital literacy', 'digital rights management', 'digital content', 'economic governance (EU)', 'economic instrument for the environment', 'inclusion in the budget', 'Institution of the Union', 'financing of the EU budget', 'competence of the institution']</t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
@@ -1239,7 +1239,7 @@
         <v>0.25</v>
       </c>
       <c r="S15" t="n">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="16">
@@ -1260,7 +1260,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>['mixed cropping', 'crop rotation', 'adaptation to climate change', 'marketing year']</t>
+          <t>['crop rotation', 'mixed cropping', 'mode of production', 'Southern neighbourhood', 'European Neighbourhood and Partnership Instrument', 'Union for the Mediterranean', 'economic instrument for the environment', 'EU strategy', 'strategic partnership (EU)', 'impact of information technology']</t>
         </is>
       </c>
       <c r="G16" t="inlineStr"/>
@@ -1311,7 +1311,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>['community resilience', 'monitoring report', 'risk management']</t>
+          <t>['monitoring report', 'disaster prevention', 'disaster management', 'resilience', 'risk assessment', 'environmental monitoring', 'data collection', 'European Union', 'implementation of EU policies', 'knowledge management']</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
@@ -1338,10 +1338,10 @@
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
       <c r="R17" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="S17" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="18">
@@ -1362,7 +1362,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>['food contact material', 'food safety']</t>
+          <t>['food contact material', 'food safety', 'food technology', 'mineral oil', 'food hygiene', 'food chain', 'food systems', 'food additive', 'food security', 'food-borne disease']</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
@@ -1392,7 +1392,7 @@
         <v>0.2</v>
       </c>
       <c r="S18" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="19">
@@ -1413,7 +1413,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>['basic education', 'special education', 'economic and social cohesion']</t>
+          <t>['special education', 'comparative education', 'cooperation in the field of education', 'inclusion in the budget', 'intercultural competences', 'democratic competences', 'social cohesion', 'active citizenship', 'pluralism in the media', 'economic and social cohesion']</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
@@ -1464,7 +1464,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>['critical infrastructure security']</t>
+          <t>['routing security', 'interoperability of networks', 'internet governance', 'information technology', 'cybersecurity', 'EU Member State', 'global network', 'adoption of standards', 'network operator', 'data analysis']</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
@@ -1494,7 +1494,7 @@
         <v>0.2</v>
       </c>
       <c r="S20" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="21">
@@ -1515,7 +1515,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>['critical infrastructure security', 'European Interoperability Framework']</t>
+          <t>['critical infrastructure security', 'EU alert system', 'area of freedom', 'security and justice', 'competence of the Member States', 'operation of the Institutions', 'primacy of EU law', 'Treaty on the Functioning of the EU', 'independence of the judiciary', 'payment system', 'liberalisation of the market']</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
@@ -1545,7 +1545,7 @@
         <v>0.2</v>
       </c>
       <c r="S21" t="n">
-        <v>0.5</v>
+        <v>0.09090909090909091</v>
       </c>
     </row>
     <row r="22">
@@ -1566,7 +1566,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>['international humanitarian law', 'aid evaluation', 'European Union Solidarity Fund', 'search and rescue']</t>
+          <t>['impact of information technology', 'degradation of the environment', 'quality of the environment', 'economic instrument for the environment', 'concentration of the population', 'composition of the population', 'Union for the Mediterranean', 'exploitation of the seas', 'freedom of the skies', 'apparatus based on the use of rays']</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
@@ -1619,7 +1619,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>['food contact material', 'EU reference laboratory', 'food safety', 'recommendation (EU)']</t>
+          <t>['mineral oil', 'food contact material', 'EU reference laboratory', 'European Union', 'EU study report', 'recommendation (EU)', 'oil refining', 'oil pollution', 'oil industry', 'edible oil']</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
@@ -1670,7 +1670,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>['research infrastructure', 'European Joint Undertaking']</t>
+          <t>['research and development', 'Joint Research Centre', 'research', 'research infrastructure', 'industrial research', 'environmental research', 'Scientific and Technical Research Committee', 'European Joint Undertaking', 'Framework Programme for Research and Development', 'think tank']</t>
         </is>
       </c>
       <c r="G24" t="inlineStr"/>
@@ -1721,7 +1721,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>['digital economy', 'digital transformation', 'clean technology', 'prospective technological studies', 'region-EU relationship']</t>
+          <t>['digital transformation', 'digital economy', 'economic and social cohesion', 'economic instrument for the environment', 'digital divide', 'smart city', 'Internet of Things', 'open science', 'EU macroregional policy', 'relations between the State and the regions']</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
@@ -1751,7 +1751,7 @@
         <v>0.2</v>
       </c>
       <c r="S25" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="26">
@@ -1772,7 +1772,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>['monitoring report', 'pollution from land-based sources', 'integrated maritime policy', 'national competent authority']</t>
+          <t>['marine litter', 'marine environment', 'environmental monitoring', 'harmonisation of legislation', 'environmental protection', 'degradation of the environment', 'exploitation of the seas', 'freedom of the seas', 'competence of the Member States', 'implementation of EU law']</t>
         </is>
       </c>
       <c r="G26" t="inlineStr"/>
@@ -1799,10 +1799,10 @@
       <c r="P26" t="inlineStr"/>
       <c r="Q26" t="inlineStr"/>
       <c r="R26" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="S26" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="27">
@@ -1823,7 +1823,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>['EU reference laboratory', 'quality control of industrial products', 'production control']</t>
+          <t>['plant health control', 'food security', 'technical standard', 'EU reference laboratory', 'novel food', 'food hygiene', 'EU study report', 'industrial research', 'economic instrument for the environment', 'quality control of industrial products']</t>
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>['renewable fuel', 'soft energy', 'water resources']</t>
+          <t>['renewable fuel', 'water', 'water management', 'water supply', 'water treatment', 'water policy', 'testing', 'degradation of the environment', 'EU strategy', 'soft energy']</t>
         </is>
       </c>
       <c r="G28" t="inlineStr"/>
@@ -1925,7 +1925,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>['waste statistics', 'hazardous waste', 'waste recycling', 'circular economy']</t>
+          <t>['hazardous waste', 'waste statistics', 'waste recycling', 'waste incineration', 'economic instrument for the environment', 'environmental tax', 'public sanitation', 'Treaty on the Functioning of the EU', 'waste management', 'environmental sustainability']</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
@@ -1952,10 +1952,10 @@
       <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr"/>
       <c r="R29" t="n">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="S29" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="30">
@@ -1976,7 +1976,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>['crisis management', 'risk management', 'disaster risk reduction']</t>
+          <t>['crisis management', 'disaster prevention', 'disaster preparedness', 'disaster response', 'risk assessment', 'satellite imagery', 'geographical information system', 'European Commission', 'interdisciplinary research', 'situational awareness']</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
@@ -2006,7 +2006,7 @@
         <v>0.2</v>
       </c>
       <c r="S30" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="31">
@@ -2027,7 +2027,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>['natural disaster', 'meteorology', 'climate security', 'adaptation to climate change', 'heatwave']</t>
+          <t>['South America', 'drought', 'America', 'Latin America', 'South-South cooperation']</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
@@ -2078,7 +2078,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>['environmental standard', 'resistance of materials', 'EU reference laboratory', 'dangerous substance']</t>
+          <t>['quality of the environment', 'degradation of the environment', 'economic instrument for the environment', 'physico-chemical property', 'safety assessment', 'nanotechnology', 'environmental impact', 'standardisation', 'laboratory test', 'OECD']</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
@@ -2105,10 +2105,10 @@
       <c r="P32" t="inlineStr"/>
       <c r="Q32" t="inlineStr"/>
       <c r="R32" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S32" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="33">
@@ -2129,7 +2129,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>['European Maritime and Fisheries Fund', 'EU strategy', 'adaptation to climate change', 'EU initiative']</t>
+          <t>['economic instrument for the environment', 'freedom of the seas', 'exploitation of the seas', 'degradation of the environment', 'quality of the environment', 'law of the sea', 'implementation of the budget', 'reform of the CAP', 'inclusion in the budget', 'relations between the State and the regions']</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
@@ -2180,7 +2180,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>['agricultural economics', 'economic accounts for agriculture', 'common agricultural policy']</t>
+          <t>['agricultural economics', 'common agricultural policy', 'economic accounts for agriculture', 'agro-industry', 'EU direct payments', 'trade agreement (EU)', 'redirection of production', 'economic governance (EU)', 'agricultural levy', 'EU initiative']</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
@@ -2210,7 +2210,7 @@
         <v>0.25</v>
       </c>
       <c r="S34" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="35">
@@ -2231,7 +2231,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>['reduction of gas emissions', 'energy market', 'energy poverty', 'building performance']</t>
+          <t>['economic instrument for the environment', 'liberalisation of the market', 'degradation of the environment', 'quality of the environment', 'quality control of industrial products', 'concentration of the population', 'composition of the population', 'coaching in the workplace', 'geographical distribution of the population', 'exploitation of the seas']</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
@@ -2258,10 +2258,10 @@
       <c r="P35" t="inlineStr"/>
       <c r="Q35" t="inlineStr"/>
       <c r="R35" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="S35" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -2282,7 +2282,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>['EU strategy', 'EU initiative']</t>
+          <t>['management committee (EU)', 'European Maritime and Fisheries Fund', 'risk management', 'advisory committee (EU)', 'management', 'technical standard', 'environmental auditing', 'economic governance (EU)', 'economic instrument for the environment', 'technical barriers to trade']</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
@@ -2333,7 +2333,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>['European Union Solidarity Fund', 'European Stability Mechanism']</t>
+          <t>['critical infrastructure security', 'industrial research', 'text and data mining', 'public policy', 'systems interconnection', 'adaptation to climate change', 'common security and defence policy', 'European Joint Undertaking', 'impact of information technology', 'services of general interest']</t>
         </is>
       </c>
       <c r="G37" t="inlineStr"/>
@@ -2360,10 +2360,10 @@
       <c r="P37" t="inlineStr"/>
       <c r="Q37" t="inlineStr"/>
       <c r="R37" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="S37" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="38">
@@ -2384,7 +2384,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>['anonymisation', 'data sharing', 'data governance', 'impact of information technology']</t>
+          <t>['data sharing', 'data governance', 'anonymisation', 'personal data', 'privacy enhancing technologies', 'impact of information technology', 'cloud computing', 'machine-readable data', 'digital infrastructure supply', 'technology transfer']</t>
         </is>
       </c>
       <c r="G38" t="inlineStr"/>
@@ -2411,10 +2411,10 @@
       <c r="P38" t="inlineStr"/>
       <c r="Q38" t="inlineStr"/>
       <c r="R38" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="S38" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="39">
@@ -2435,7 +2435,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>['European Union Solidarity Fund', 'EU macroregional policy']</t>
+          <t>['European Union', 'drought', 'Northern Europe', 'Southern Europe', 'Europe', 'European Union Solidarity Fund', 'economic instrument for the environment', 'member country', 'adverse climatic event', 'seasonal forecast']</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
@@ -2462,10 +2462,10 @@
       <c r="P39" t="inlineStr"/>
       <c r="Q39" t="inlineStr"/>
       <c r="R39" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S39" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="40">
@@ -2486,7 +2486,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>['reduction of gas emissions', 'Paris Agreement on Climate Change']</t>
+          <t>['reduction of gas emissions', 'carbon neutrality', 'emission trading', 'emission allowance', 'clean development mechanism', 'land use', 'Paris Agreement on Climate Change', 'Kyoto Protocol', 'carbon capture and storage', 'EU Emissions Trading Scheme']</t>
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
@@ -2516,7 +2516,7 @@
         <v>0.5</v>
       </c>
       <c r="S40" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="41">
@@ -2537,7 +2537,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>['adaptation to climate change', 'Health Emergency Preparedness and Response Authority', 'European Health Union']</t>
+          <t>['economic instrument for the environment', 'degradation of the environment', 'quality of the environment', 'Health Emergency Preparedness and Response Authority', 'circular economy', 'public health', 'epidemiology', 'environmental risk', 'resilience of the economy', 'social inequality']</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
@@ -2564,10 +2564,10 @@
       <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr"/>
       <c r="R41" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S41" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="42">
@@ -2588,7 +2588,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>['critical infrastructure security', 'community resilience']</t>
+          <t>['load', 'damage', 'assessment', 'evaluation method', 'critical infrastructure security', 'disaster risk reduction', 'war damage', 'technology assessment', 'industrial structures', 'protection of communications']</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
@@ -2639,7 +2639,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>['EU study report', 'recommendation (EU)']</t>
+          <t>['paints and varnishes', 'EU study report', 'economic instrument for the environment', 'recommendation (EU)', 'EU activity', 'expert group (EU)', 'economic and social cohesion']</t>
         </is>
       </c>
       <c r="G43" t="inlineStr"/>
@@ -2690,7 +2690,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>['carbon neutrality', 'sustainable finance', 'macroeconomics']</t>
+          <t>['alternative investment', 'carbon neutrality', 'sustainable finance', 'gross domestic product', 'EU financial instrument', 'data science', 'data sharing', 'public data', 'carbon capture and storage', 'open data']</t>
         </is>
       </c>
       <c r="G44" t="inlineStr"/>
@@ -2741,7 +2741,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>['disruptive technology', 'quantum technology', 'EU strategy']</t>
+          <t>['disruptive technology', 'quantum technology', 'astronautics', 'foresight', 'EU study report', 'dual-use technology', 'common security and defence policy', 'EU strategy', 'strategic partnership (EU)', 'European Union']</t>
         </is>
       </c>
       <c r="G45" t="inlineStr"/>
@@ -2792,7 +2792,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>['innovation', 'research infrastructure', 'knowledge economy', 'smart specialisation']</t>
+          <t>['innovation', 'research infrastructure', 'open innovation', 'knowledge economy', 'EU study report', 'value chain', 'economic geography', 'economic value', 'services of general interest', 'impact of information technology']</t>
         </is>
       </c>
       <c r="G46" t="inlineStr"/>
@@ -2819,10 +2819,10 @@
       <c r="P46" t="inlineStr"/>
       <c r="Q46" t="inlineStr"/>
       <c r="R46" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="S46" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="47">
@@ -2843,7 +2843,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>['forced migration', 'spatial data', 'adaptation to climate change', 'natural disaster']</t>
+          <t>['forced migration', 'migration', 'environmental risk prevention', 'spatial data', 'public data', 'data science', 'environmental cooperation', 'open data', 'satellite data', 'environmental conditions']</t>
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
@@ -2870,10 +2870,10 @@
       <c r="P47" t="inlineStr"/>
       <c r="Q47" t="inlineStr"/>
       <c r="R47" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="S47" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -2894,7 +2894,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>['emission trading', 'land use', 'Kyoto Protocol', 'economic instrument for the environment']</t>
+          <t>['land use', 'public-private partnership', 'emission trading', 'pollution from land-based sources', 'economic instrument for the environment', 'Kyoto Protocol', 'reduction of gas emissions', 'EU study report', 'public goods', 'economic governance (EU)']</t>
         </is>
       </c>
       <c r="G48" t="inlineStr"/>
@@ -2921,10 +2921,10 @@
       <c r="P48" t="inlineStr"/>
       <c r="Q48" t="inlineStr"/>
       <c r="R48" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="S48" t="n">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="49">
@@ -2945,7 +2945,7 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>['renewable fuel', 'substitute fuel']</t>
+          <t>['renewable fuel', 'substitute fuel', 'energy market', 'clean technology', 'energy transition', 'solar energy', 'regulation (EU)', 'ecodesign', 'technology transfer', 'intermediate technology']</t>
         </is>
       </c>
       <c r="G49" t="inlineStr"/>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>['financial stability', 'EU financing', 'EU financial instrument']</t>
+          <t>['aid evaluation', 'control of State aid', 'financial stability', 'EU initiative', 'economic instrument for the environment', 'Treaty on the Functioning of the EU', 'relations between the State and the regions', 'balance of payments assistance', 'financing of the EU budget', 'EU strategy']</t>
         </is>
       </c>
       <c r="G50" t="inlineStr"/>
@@ -3048,7 +3048,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>['nature restoration', 'carbon capture and storage', 'EU strategy', 'remote sensing']</t>
+          <t>['forest', 'carbon capture and storage', 'nature restoration', 'EU strategy', 'forest certification', 'open data', 'text and data mining', 'economic instrument for the environment', 'public data', 'management information system']</t>
         </is>
       </c>
       <c r="G51" t="inlineStr"/>
@@ -3099,7 +3099,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>['business-to-consumer', 'smart technology', 'quality control of industrial products', 'multilateral surveillance']</t>
+          <t>['competence of the Member States', 'business-to-consumer', 'liberalisation of the market', 'quality of the environment', 'economic instrument for the environment', 'consumer organisations', 'artificial intelligence', 'single market', 'monitoring system', 'Member States']</t>
         </is>
       </c>
       <c r="G52" t="inlineStr"/>
@@ -3150,7 +3150,7 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>['biodiversity', 'agroforestry', 'land use', 'plantation']</t>
+          <t>['biodiversity', 'land use', 'agroforestry', 'cocoa', 'land governance', 'nature restoration', 'land reform', 'food systems', 'pollution from land-based sources', 'ecological tourism']</t>
         </is>
       </c>
       <c r="G53" t="inlineStr"/>
@@ -3180,7 +3180,7 @@
         <v>0.3333333333333333</v>
       </c>
       <c r="S53" t="n">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="54">
@@ -3201,7 +3201,7 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>['authorised catch', 'monitoring report']</t>
+          <t>['common fisheries policy', 'Protocol (EU)', 'fisheries policy', 'European Maritime and Fisheries Fund', 'exploitation of the seas', 'economic instrument for the environment', 'policy analysis', 'Treaty on the Functioning of the EU', 'EU policy - national policy', 'degradation of the environment']</t>
         </is>
       </c>
       <c r="G54" t="inlineStr"/>
@@ -3254,7 +3254,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>['reduction of gas emissions', 'Paris Agreement on Climate Change', 'energy transition', 'sustainable finance']</t>
+          <t>['Paris Agreement on Climate Change', 'energy transition', 'reduction of gas emissions', 'adaptation to climate change', 'economic instrument for the environment', 'energy market', 'sustainable finance', 'energy audit', 'climate security', 'carbon capture and storage']</t>
         </is>
       </c>
       <c r="G55" t="inlineStr"/>
@@ -3305,7 +3305,7 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>['heatwave', 'adaptation to climate change', 'natural disaster', 'meteorology']</t>
+          <t>['degradation of the environment', 'quality of the environment', 'concentration of the population', 'composition of the population', 'economic instrument for the environment', 'evacuation of the population']</t>
         </is>
       </c>
       <c r="G56" t="inlineStr"/>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>['impact of information technology', '5G', 'ecodesign']</t>
+          <t>['economic instrument for the environment', 'degradation of the environment', 'quality of the environment', 'Internet of Things', 'liberalisation of the market', 'telecommunications', 'sustainability', 'environmental impact', 'digital technology', 'energy efficiency']</t>
         </is>
       </c>
       <c r="G57" t="inlineStr"/>
@@ -3408,7 +3408,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>['adaptation to climate change', 'carbon neutrality', 'reduction of gas emissions', 'carbon capture and storage', 'bioclimatology']</t>
+          <t>['climate change', 'climate change policy', 'adaptation to climate change', 'carbon', 'carbon neutrality', 'carbon capture and storage', 'reduction of gas emissions', 'forest', 'economic instrument for the environment', 'final consumption']</t>
         </is>
       </c>
       <c r="G58" t="inlineStr"/>
@@ -3438,7 +3438,7 @@
         <v>0.1666666666666667</v>
       </c>
       <c r="S58" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="59">
@@ -3459,7 +3459,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>['open data', 'industrial research', 'data sharing', 'data governance']</t>
+          <t>['economic instrument for the environment', 'quality control of industrial products', 'text and data mining', 'systems interconnection', 'degradation of the environment', 'liberalisation of the market', 'impact of information technology', 'inclusion in the budget', 'right to development', 'exploitation of the seas']</t>
         </is>
       </c>
       <c r="G59" t="inlineStr"/>
@@ -3510,7 +3510,7 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>['mixed cropping', 'crop rotation', 'heatwave']</t>
+          <t>['crop yield', 'European Neighbourhood and Partnership Instrument', 'Southern neighbourhood', 'marketing year', 'fallow', 'crop rotation', 'mixed cropping', 'heatwave', 'economic accounts for agriculture', 'Union for the Mediterranean']</t>
         </is>
       </c>
       <c r="G60" t="inlineStr"/>
@@ -3561,7 +3561,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>['silo', 'agricultural area with environmental restrictions', 'fallow', 'mixed cropping']</t>
+          <t>['European Neighbourhood and Partnership Instrument', 'European Union', 'Southern neighbourhood', 'Russia', 'crop monitoring', 'winter cereals', 'spring cereals', 'grain maize', 'unfavourable weather', 'agricultural production.']</t>
         </is>
       </c>
       <c r="G61" t="inlineStr"/>

</xml_diff>

<commit_message>
Creating hybrid search SBERT branch
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -543,7 +543,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>['resistance of materials', 'energy audit', 'building performance']</t>
+          <t>['building regulations', 'building materials', 'building technique', 'architectural heritage', 'building safety', 'resistance of materials', 'building performance', 'seismic monitoring', 'improvement of housing', 'energy research']</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
@@ -590,7 +590,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>['smart city', 'Internet of Things', 'smart technology', 'prospective technological studies', 'smart specialisation']</t>
+          <t>['smart city', 'smart technology', 'scientific research', 'intellectual property', 'industrial research', 'technological process', 'bibliometry', 'urban infrastructure', 'technological change', 'prospective technological studies']</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -641,7 +641,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>['adaptation to climate change', 'climate security', 'natural disaster', 'crisis management', 'geographical information system']</t>
+          <t>['adaptation to climate change', 'crisis management', 'natural disaster', 'satellite data', 'climate change', 'earth observation', 'meteorology', 'aid to disaster victims', 'disaster risk reduction', 'space research']</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
@@ -668,10 +668,10 @@
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr"/>
       <c r="R4" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S4" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="5">
@@ -698,7 +698,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>['adaptation to climate change', 'community resilience', 'citizen science', 'natural disaster', 'popularising science']</t>
+          <t>['natural disaster', 'disaster risk reduction', 'risk management', 'hazard science', 'climate security', 'adaptation to climate change', 'environmental risk prevention', 'knowledge management', 'humanitarian crisis', 'foresight']</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
@@ -725,10 +725,10 @@
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="S5" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="6">
@@ -749,7 +749,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>['municipal waste', 'waste recycling', 'circular economy']</t>
+          <t>['waste recycling', 'municipal waste', 'circular economy', 'packaging product', 'waste disposal', 'labelling', 'waste management', 'eco-label', 'packaging', 'recycled product']</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
@@ -776,10 +776,10 @@
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="S6" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="7">
@@ -800,7 +800,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>['data sharing', 'European Interoperability Framework', 'systems interconnection', 'data governance']</t>
+          <t>['data sharing', 'spatial data', 'European Interoperability Framework', 'systems interconnection', 'technical standard', 'geographical information system', 'cross-frontier data flow', 'public data', 'open data', 'technical barriers to trade']</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
@@ -827,10 +827,10 @@
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S7" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="8">
@@ -851,7 +851,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>['EU study report', 'EU reference laboratory']</t>
+          <t>['European Commission', 'EU competence', 'EU study report', 'competence of the institution', 'EU programme', 'aid evaluation', 'EU institution', 'microeconomics', 'data governance', 'powers of the institutions (EU)']</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
@@ -878,10 +878,10 @@
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
       <c r="R8" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="S8" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="9">
@@ -903,7 +903,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>['quality standard', 'ecodesign']</t>
+          <t>['energy storage', 'electricity storage device', 'energy efficiency', 'environmental standard', 'energy research', 'energy technology', 'quality standard', 'ecodesign', 'energy use', 'renewable energy']</t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
@@ -954,7 +954,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>['EU study report', 'EU policy - national policy', 'prospective technological studies']</t>
+          <t>['smart technology', 'prospective technological studies', 'EU industrial policy', 'automation', 'policy analysis', 'robotisation', 'EU research policy', 'European industrial area', 'industrial robot', 'knowledge economy']</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
@@ -981,10 +981,10 @@
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
       <c r="R10" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S10" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="11">
@@ -1005,7 +1005,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>['supply chain', 'raw material', 'terms of trade', 'EU market']</t>
+          <t>['trade relations', 'foreign trade', 'extra-EU trade', 'international trade', 'trade by country', 'raw material', 'supply chain', 'trade information', 'Kazakhstan', 'value chain']</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
@@ -1032,10 +1032,10 @@
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
       <c r="R11" t="n">
-        <v>0.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="S11" t="n">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="12">
@@ -1056,7 +1056,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>['crop rotation', 'agricultural economics', 'precision agriculture']</t>
+          <t>['crop yield', 'crop production', 'crop losses', 'Tunisia', 'Mediterranean agriculture', 'Southern neighbourhood', 'agricultural region', 'Algeria', 'Morocco', 'Libya']</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
@@ -1083,10 +1083,10 @@
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr"/>
       <c r="R12" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="S12" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="13">
@@ -1107,7 +1107,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>['smart technology', 'European Interoperability Framework', 'systems interconnection']</t>
+          <t>['smart technology', 'systems interconnection', 'Internet of Things', 'energy grid', 'household electrical appliance', 'energy policy', 'energy market', 'energy technology', 'EU energy policy', 'ecodesign']</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
@@ -1137,7 +1137,7 @@
         <v>0.25</v>
       </c>
       <c r="S13" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="14">
@@ -1158,7 +1158,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>['aviation security', 'critical infrastructure security', 'drone']</t>
+          <t>['critical infrastructure security', 'aviation security', 'drone', 'building safety', 'threat to national security', 'protective equipment', 'protected area', 'anti-missile defence', 'building regulations', 'military equipment']</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
@@ -1188,7 +1188,7 @@
         <v>0.4</v>
       </c>
       <c r="S14" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="15">
@@ -1209,7 +1209,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>['digital transformation', 'impact of information technology', 'economic intelligence', 'economic governance (EU)']</t>
+          <t>['digital transformation', 'impact of information technology', 'digital economy', 'prospective technological studies', 'digital technology', 'knowledge economy', 'technological change', 'globalisation', 'information society', 'technology assessment']</t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
@@ -1236,10 +1236,10 @@
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
       <c r="R15" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="S15" t="n">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="16">
@@ -1260,7 +1260,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>['mixed cropping', 'crop rotation', 'adaptation to climate change', 'marketing year']</t>
+          <t>['Ukraine', 'crop yield', 'crop production', 'winter crop', 'cereal-growing', 'agricultural situation', 'climatic zone', 'agricultural statistics', 'agricultural region', 'Southern neighbourhood']</t>
         </is>
       </c>
       <c r="G16" t="inlineStr"/>
@@ -1287,10 +1287,10 @@
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
       <c r="R16" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="S16" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="17">
@@ -1311,7 +1311,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>['community resilience', 'monitoring report', 'risk management']</t>
+          <t>['monitoring report', 'disaster risk reduction', 'natural disaster', 'risk management', 'crisis management', 'EU alert system', 'disaster area', 'humanitarian crisis', 'data governance', 'hazard science']</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
@@ -1338,10 +1338,10 @@
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
       <c r="R17" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S17" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="18">
@@ -1362,7 +1362,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>['food contact material', 'food safety']</t>
+          <t>['food contact material', 'mineral oil', 'food safety', 'food contamination', 'food chemistry', 'hydrocarbon', 'food inspection', 'food standard', 'petroleum product', 'food hygiene']</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
@@ -1389,10 +1389,10 @@
       <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr"/>
       <c r="R18" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="S18" t="n">
         <v>0.2</v>
-      </c>
-      <c r="S18" t="n">
-        <v>0.5</v>
       </c>
     </row>
     <row r="19">
@@ -1413,7 +1413,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>['basic education', 'special education', 'economic and social cohesion']</t>
+          <t>['special education', 'democratisation of education', 'European citizenship', 'education of foreigners', 'EU initiative', 'comparative education', 'European Union', 'inclusion in the budget', 'social dialogue (EU)', 'intercultural competences']</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
@@ -1464,7 +1464,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>['critical infrastructure security']</t>
+          <t>['critical infrastructure security', 'international security', 'European security', 'harmonisation of standards', 'safety standard', 'information security', 'international standard', 'European Interoperability Framework', 'protection of communications', 'European standard']</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
@@ -1494,7 +1494,7 @@
         <v>0.2</v>
       </c>
       <c r="S20" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="21">
@@ -1515,7 +1515,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>['critical infrastructure security', 'European Interoperability Framework']</t>
+          <t>['critical infrastructure security', 'European Union Agency for Cybersecurity', 'European security', 'information security', 'data governance', 'European Interoperability Framework', 'international security', 'dissemination of EU information', 'Body of European Regulators for Electronic Communications', 'extranet']</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
@@ -1545,7 +1545,7 @@
         <v>0.2</v>
       </c>
       <c r="S21" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="22">
@@ -1566,7 +1566,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>['international humanitarian law', 'aid evaluation', 'European Union Solidarity Fund', 'search and rescue']</t>
+          <t>['earthquake', 'Türkiye', 'Syria', 'humanitarian crisis', 'seismic monitoring', 'geophysical environment', 'satellite data', 'humanitarian aid', 'disaster area', 'European Space Agency']</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
@@ -1593,10 +1593,10 @@
       <c r="P22" t="inlineStr"/>
       <c r="Q22" t="inlineStr"/>
       <c r="R22" t="n">
-        <v>0</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="S22" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="23">
@@ -1619,7 +1619,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>['food contact material', 'EU reference laboratory', 'food safety', 'recommendation (EU)']</t>
+          <t>['mineral oil', 'food contact material', 'vegetable oil', 'food hygiene', 'EU reference laboratory', 'hydrocarbon', 'food chemistry', 'food inspection', 'petroleum product', 'storage of hydrocarbons']</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
@@ -1670,7 +1670,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>['research infrastructure', 'European Joint Undertaking']</t>
+          <t>['Joint Research Centre', 'research and development', 'research infrastructure', 'industrial research', 'European association', 'scientific committee (EU)', 'Framework Programme for Research and Development', 'European Union Institute for Security Studies', 'economic and social cohesion', 'European Centre for Parliamentary Research and Documentation']</t>
         </is>
       </c>
       <c r="G24" t="inlineStr"/>
@@ -1721,7 +1721,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>['digital economy', 'digital transformation', 'clean technology', 'prospective technological studies', 'region-EU relationship']</t>
+          <t>['digital technology', 'European patent', 'clean technology', 'technological change', 'technological independence', 'digital transformation', 'technology transfer', 'European industrial area', 'prospective technological studies', 'EU research policy']</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
@@ -1748,7 +1748,7 @@
       <c r="P25" t="inlineStr"/>
       <c r="Q25" t="inlineStr"/>
       <c r="R25" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="S25" t="n">
         <v>0.2</v>
@@ -1772,7 +1772,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>['monitoring report', 'pollution from land-based sources', 'integrated maritime policy', 'national competent authority']</t>
+          <t>['marine pollution', 'marine ecosystem', 'marine environment', 'environmental monitoring', 'coastal pollution', 'EU environmental policy', 'marine life', 'integrated maritime policy', 'coastal protection', 'environmental indicator']</t>
         </is>
       </c>
       <c r="G26" t="inlineStr"/>
@@ -1799,10 +1799,10 @@
       <c r="P26" t="inlineStr"/>
       <c r="Q26" t="inlineStr"/>
       <c r="R26" t="n">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="S26" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="27">
@@ -1823,7 +1823,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>['EU reference laboratory', 'quality control of industrial products', 'production control']</t>
+          <t>['genetically modified organism', 'food safety', 'foodstuffs legislation', 'genetic engineering', 'biotechnology', 'transgenic plant', 'crop production', 'agricultural product', 'quality control of agricultural products', 'EU reference laboratory']</t>
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
@@ -1850,10 +1850,10 @@
       <c r="P27" t="inlineStr"/>
       <c r="Q27" t="inlineStr"/>
       <c r="R27" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S27" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="28">
@@ -1874,7 +1874,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>['renewable fuel', 'soft energy', 'water resources']</t>
+          <t>['renewable energy', 'hydrogen', 'hydrogen production', 'electrochemistry', 'renewable fuel', 'water', 'electrical engineering', 'electrotechnology', 'energy industry', 'solar energy end-use applications']</t>
         </is>
       </c>
       <c r="G28" t="inlineStr"/>
@@ -1901,10 +1901,10 @@
       <c r="P28" t="inlineStr"/>
       <c r="Q28" t="inlineStr"/>
       <c r="R28" t="n">
-        <v>0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="S28" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="29">
@@ -1925,7 +1925,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>['waste statistics', 'hazardous waste', 'waste recycling', 'circular economy']</t>
+          <t>['waste recycling', 'waste management', 'waste incineration', 'hazardous waste', 'circular economy', 'substitute fuel', 'oil refining', 'waste statistics', 'petroleum product', 'sustainable product']</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
@@ -1955,7 +1955,7 @@
         <v>0.5</v>
       </c>
       <c r="S29" t="n">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="30">
@@ -1976,7 +1976,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>['crisis management', 'risk management', 'disaster risk reduction']</t>
+          <t>['crisis management', 'risk management', 'disaster risk reduction', 'natural disaster', 'humanitarian crisis', 'hazard science', 'disaster area', 'community resilience', 'EU alert system', 'monitoring report']</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
@@ -2006,7 +2006,7 @@
         <v>0.2</v>
       </c>
       <c r="S30" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="31">
@@ -2027,7 +2027,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>['natural disaster', 'meteorology', 'climate security', 'adaptation to climate change', 'heatwave']</t>
+          <t>['South America', 'drought', 'heatwave', 'climate', 'climate change', 'natural disaster', 'atmospheric conditions', 'arid zone', 'adaptation to climate change', 'global warming']</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
@@ -2078,7 +2078,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>['environmental standard', 'resistance of materials', 'EU reference laboratory', 'dangerous substance']</t>
+          <t>['nanotechnology', 'hydrophobicity', 'environmental standard', 'dangerous substance', 'biochemistry', 'biomaterials', 'quality of the environment', 'chemicals legislation', 'biological standard', 'water protection']</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
@@ -2105,10 +2105,10 @@
       <c r="P32" t="inlineStr"/>
       <c r="Q32" t="inlineStr"/>
       <c r="R32" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S32" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="33">
@@ -2129,7 +2129,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>['European Maritime and Fisheries Fund', 'EU strategy', 'adaptation to climate change', 'EU initiative']</t>
+          <t>['marine ecosystem', 'marine environment', 'EU environmental policy', 'adaptation to climate change', 'exploitation of the seas', 'aquatic ecosystem', 'marine pollution', 'EU strategy', 'sustainable fisheries', 'common fisheries policy']</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
@@ -2156,10 +2156,10 @@
       <c r="P33" t="inlineStr"/>
       <c r="Q33" t="inlineStr"/>
       <c r="R33" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S33" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="34">
@@ -2180,7 +2180,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>['agricultural economics', 'economic accounts for agriculture', 'common agricultural policy']</t>
+          <t>['agricultural statistics', 'agricultural economics', 'EU agricultural market', 'agricultural trade', 'agricultural production', 'agricultural surplus', 'supply balance sheet', 'agricultural policy', 'agricultural production policy', 'agricultural product']</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
@@ -2207,10 +2207,10 @@
       <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr"/>
       <c r="R34" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="S34" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="35">
@@ -2231,7 +2231,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>['reduction of gas emissions', 'energy market', 'energy poverty', 'building performance']</t>
+          <t>['heat pump', 'energy grid', 'energy poverty', 'refrigeration industry', 'renewable energy', 'heating', 'energy policy', 'energy technology', 'household electrical appliance', 'ecodesign']</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
@@ -2258,10 +2258,10 @@
       <c r="P35" t="inlineStr"/>
       <c r="Q35" t="inlineStr"/>
       <c r="R35" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="S35" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -2282,7 +2282,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>['EU strategy', 'EU initiative']</t>
+          <t>['fishery management', 'sustainable fisheries', 'common fisheries policy', 'fisheries policy', 'scientific committee (EU)', 'fishery research', 'fishery resources', 'conservation of fish stocks', 'fishing regulations', 'authorised catch']</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
@@ -2309,10 +2309,10 @@
       <c r="P36" t="inlineStr"/>
       <c r="Q36" t="inlineStr"/>
       <c r="R36" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S36" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="37">
@@ -2333,7 +2333,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>['European Union Solidarity Fund', 'European Stability Mechanism']</t>
+          <t>['EU initiative', 'EC Regulation', 'text and data mining', 'area of freedom', 'security and justice', 'European Union Solidarity Fund', 'impact of information technology', 'search and rescue', 'common security and defence policy', 'European Union Agency for Cybersecurity', 'technical committee (EU)']</t>
         </is>
       </c>
       <c r="G37" t="inlineStr"/>
@@ -2384,7 +2384,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>['anonymisation', 'data sharing', 'data governance', 'impact of information technology']</t>
+          <t>['data sharing', 'anonymisation', 'data protection', 'protection of privacy', 'personal data', 'information security', 'confidentiality', 'impact of information technology', 'data governance', 'digital rights management']</t>
         </is>
       </c>
       <c r="G38" t="inlineStr"/>
@@ -2411,10 +2411,10 @@
       <c r="P38" t="inlineStr"/>
       <c r="Q38" t="inlineStr"/>
       <c r="R38" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S38" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="39">
@@ -2435,7 +2435,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>['European Union Solidarity Fund', 'EU macroregional policy']</t>
+          <t>['drought', 'Northern Europe', 'Southern Europe', 'Europe', 'climate', 'climate change', 'adaptation to climate change', 'EU environmental policy', 'Mediterranean region (EU)', 'climatic zone']</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
@@ -2462,10 +2462,10 @@
       <c r="P39" t="inlineStr"/>
       <c r="Q39" t="inlineStr"/>
       <c r="R39" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S39" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="40">
@@ -2486,7 +2486,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>['reduction of gas emissions', 'Paris Agreement on Climate Change']</t>
+          <t>['greenhouse gas', 'Paris Agreement on Climate Change', 'environmental statistics', 'international statistics', 'global warming', 'environmental monitoring', 'atmospheric pollutant', 'land use', 'environmental indicator', 'UN Framework Convention on Climate Change']</t>
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
@@ -2513,10 +2513,10 @@
       <c r="P40" t="inlineStr"/>
       <c r="Q40" t="inlineStr"/>
       <c r="R40" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="S40" t="n">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="41">
@@ -2537,7 +2537,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>['adaptation to climate change', 'Health Emergency Preparedness and Response Authority', 'European Health Union']</t>
+          <t>['climate change', 'environmental protection', 'environmental risk prevention', 'nanotechnology', 'environmental impact', 'EU environmental policy', 'economic instrument for the environment', 'disaster risk reduction', 'circular economy', 'public health.']</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
@@ -2588,7 +2588,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>['critical infrastructure security', 'community resilience']</t>
+          <t>['damage', 'blast protection', 'critical infrastructure security', 'evaluation method', 'building safety', 'load', 'assessment', 'explosive', 'protective equipment', 'industrial structures']</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
@@ -2615,10 +2615,10 @@
       <c r="P42" t="inlineStr"/>
       <c r="Q42" t="inlineStr"/>
       <c r="R42" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S42" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="43">
@@ -2639,7 +2639,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>['EU study report', 'recommendation (EU)']</t>
+          <t>['paints and varnishes', 'eco-label', 'environmental standard', 'EU environmental policy', 'dangerous substance', 'biocide', 'chemicals legislation', 'derogation from EU law', 'toxic substance', 'chemical pollution']</t>
         </is>
       </c>
       <c r="G43" t="inlineStr"/>
@@ -2690,7 +2690,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>['carbon neutrality', 'sustainable finance', 'macroeconomics']</t>
+          <t>['carbon neutrality', 'macroeconomics', 'EU investment', 'industrial investment', 'EU energy policy', 'regulation of investments', 'investment cost', 'data science', 'EU growth strategy', 'alternative investment']</t>
         </is>
       </c>
       <c r="G44" t="inlineStr"/>
@@ -2741,7 +2741,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>['disruptive technology', 'quantum technology', 'EU strategy']</t>
+          <t>['foresight', 'disruptive technology', 'space technology', 'prospective technological studies', 'EU strategy', 'dual-use technology', 'nuclear technology', 'space policy', 'European defence policy', 'quantum technology']</t>
         </is>
       </c>
       <c r="G45" t="inlineStr"/>
@@ -2768,10 +2768,10 @@
       <c r="P45" t="inlineStr"/>
       <c r="Q45" t="inlineStr"/>
       <c r="R45" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S45" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="46">
@@ -2792,7 +2792,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>['innovation', 'research infrastructure', 'knowledge economy', 'smart specialisation']</t>
+          <t>['innovation', 'open innovation', 'research infrastructure', 'business cluster', 'technology park', 'organisation of research', 'knowledge economy', 'smart specialisation', 'value chain', 'diffusion of innovations']</t>
         </is>
       </c>
       <c r="G46" t="inlineStr"/>
@@ -2819,10 +2819,10 @@
       <c r="P46" t="inlineStr"/>
       <c r="Q46" t="inlineStr"/>
       <c r="R46" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="S46" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="47">
@@ -2843,7 +2843,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>['forced migration', 'spatial data', 'adaptation to climate change', 'natural disaster']</t>
+          <t>['forced migration', 'natural disaster', 'migration', 'migration statistics', 'spatial data', 'internally displaced person', 'migratory movement', 'disaster risk reduction', 'environmental cost', 'adaptation to climate change']</t>
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
@@ -2870,10 +2870,10 @@
       <c r="P47" t="inlineStr"/>
       <c r="Q47" t="inlineStr"/>
       <c r="R47" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="S47" t="n">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="48">
@@ -2894,7 +2894,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>['emission trading', 'land use', 'Kyoto Protocol', 'economic instrument for the environment']</t>
+          <t>['land use', 'EU Emissions Trading Scheme', 'emission trading', 'reduction of gas emissions', 'greenhouse gas', 'environmental policy', 'land policies', 'pollution from land-based sources', 'private sector', 'Paris Agreement on Climate Change']</t>
         </is>
       </c>
       <c r="G48" t="inlineStr"/>
@@ -2921,10 +2921,10 @@
       <c r="P48" t="inlineStr"/>
       <c r="Q48" t="inlineStr"/>
       <c r="R48" t="n">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="S48" t="n">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="49">
@@ -2945,7 +2945,7 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>['renewable fuel', 'substitute fuel']</t>
+          <t>['renewable fuel', 'solar energy', 'renewable energy', 'energy technology', 'carbon neutrality', 'clean technology', 'energy production', 'energy transition', 'energy market', 'renewable resources']</t>
         </is>
       </c>
       <c r="G49" t="inlineStr"/>
@@ -2972,10 +2972,10 @@
       <c r="P49" t="inlineStr"/>
       <c r="Q49" t="inlineStr"/>
       <c r="R49" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S49" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="50">
@@ -2996,7 +2996,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>['financial stability', 'EU financing', 'EU financial instrument']</t>
+          <t>['State aid', 'aid to industry', 'economic aid', 'company in difficulties', 'financing of aid', 'support mechanism', 'control of State aid', 'private-sector liquidity', 'aid evaluation', 'investment aid']</t>
         </is>
       </c>
       <c r="G50" t="inlineStr"/>
@@ -3023,10 +3023,10 @@
       <c r="P50" t="inlineStr"/>
       <c r="Q50" t="inlineStr"/>
       <c r="R50" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="S50" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="51">
@@ -3048,7 +3048,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>['nature restoration', 'carbon capture and storage', 'EU strategy', 'remote sensing']</t>
+          <t>['forest', 'nature restoration', 'sustainable forest management', 'European forestry policy', 'forestry research', 'forestry statistics', 'carbon capture and storage', 'EU environmental policy', 'reduction of gas emissions', 'conservation of resources']</t>
         </is>
       </c>
       <c r="G51" t="inlineStr"/>
@@ -3075,10 +3075,10 @@
       <c r="P51" t="inlineStr"/>
       <c r="Q51" t="inlineStr"/>
       <c r="R51" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="S51" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="52">
@@ -3099,7 +3099,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>['business-to-consumer', 'smart technology', 'quality control of industrial products', 'multilateral surveillance']</t>
+          <t>["'product quality'", "'food inspection'", "'public awareness campaign'", "'consumer information'", "'consumer goods'", "'mobile application'", "'citizen science'", "'consumer behaviour'", "'packaging product'", "'processed food product'"]</t>
         </is>
       </c>
       <c r="G52" t="inlineStr"/>
@@ -3150,7 +3150,7 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>['biodiversity', 'agroforestry', 'land use', 'plantation']</t>
+          <t>['biodiversity', 'land use', 'agroforestry', 'agricultural land', 'environmental impact', 'deforestation', 'sustainable agriculture', 'tropical agriculture', 'plantation', 'terrestrial ecosystem']</t>
         </is>
       </c>
       <c r="G53" t="inlineStr"/>
@@ -3177,10 +3177,10 @@
       <c r="P53" t="inlineStr"/>
       <c r="Q53" t="inlineStr"/>
       <c r="R53" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="S53" t="n">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="54">
@@ -3201,7 +3201,7 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>['authorised catch', 'monitoring report']</t>
+          <t>['common fisheries policy', 'fisheries policy', 'sustainable fisheries', 'monitoring report', 'fishery management', 'fishing regulations', 'fishery resources', 'fishing controls', 'fishing statistics', 'authorised catch']</t>
         </is>
       </c>
       <c r="G54" t="inlineStr"/>
@@ -3254,7 +3254,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>['reduction of gas emissions', 'Paris Agreement on Climate Change', 'energy transition', 'sustainable finance']</t>
+          <t>['Paris Agreement on Climate Change', 'energy transition', 'reduction of gas emissions', 'climate change policy', 'carbon neutrality', 'energy production', 'energy demand', 'renewable energy', 'UN Framework Convention on Climate Change', 'global warming']</t>
         </is>
       </c>
       <c r="G55" t="inlineStr"/>
@@ -3281,10 +3281,10 @@
       <c r="P55" t="inlineStr"/>
       <c r="Q55" t="inlineStr"/>
       <c r="R55" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S55" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="56">
@@ -3305,7 +3305,7 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>['heatwave', 'adaptation to climate change', 'natural disaster', 'meteorology']</t>
+          <t>['drought', 'heatwave', 'South America', 'climate', 'climate change', 'adaptation to climate change', 'tropical zone', 'tropical forest', 'atmospheric conditions', 'global warming']</t>
         </is>
       </c>
       <c r="G56" t="inlineStr"/>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>['impact of information technology', '5G', 'ecodesign']</t>
+          <t>['ecological footprint', 'environmental indicator', 'environmental impact', 'environmental protection', 'telecommunications policy', 'telecommunications industry', 'telecommunications equipment', 'digital infrastructure supply', 'regulation of telecommunications', 'environmental monitoring']</t>
         </is>
       </c>
       <c r="G57" t="inlineStr"/>
@@ -3384,10 +3384,10 @@
       <c r="P57" t="inlineStr"/>
       <c r="Q57" t="inlineStr"/>
       <c r="R57" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="S57" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="58">
@@ -3408,7 +3408,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>['adaptation to climate change', 'carbon neutrality', 'reduction of gas emissions', 'carbon capture and storage', 'bioclimatology']</t>
+          <t>['climate change', 'climate change policy', 'sustainable forest management', 'forest conservation', 'forest', 'wood production', 'European forestry policy', 'forestry research', 'carbon neutrality', 'reduction of gas emissions']</t>
         </is>
       </c>
       <c r="G58" t="inlineStr"/>
@@ -3438,7 +3438,7 @@
         <v>0.1666666666666667</v>
       </c>
       <c r="S58" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="59">
@@ -3459,7 +3459,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>['open data', 'industrial research', 'data sharing', 'data governance']</t>
+          <t>['data sharing', 'open data', 'data governance', 'data collection', 'industrial data processing', 'hydrogen production', 'sustainable product', 'product life', 'eco-design', 'economic instrument for the environment']</t>
         </is>
       </c>
       <c r="G59" t="inlineStr"/>
@@ -3486,10 +3486,10 @@
       <c r="P59" t="inlineStr"/>
       <c r="Q59" t="inlineStr"/>
       <c r="R59" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="S59" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="60">
@@ -3510,7 +3510,7 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>['mixed cropping', 'crop rotation', 'heatwave']</t>
+          <t>['crop yield', 'crop production', 'Türkiye', 'agricultural situation', 'agricultural performance', 'agricultural productivity', 'Mediterranean agriculture', 'agricultural region', 'sustainable agriculture', 'wheat']</t>
         </is>
       </c>
       <c r="G60" t="inlineStr"/>
@@ -3537,10 +3537,10 @@
       <c r="P60" t="inlineStr"/>
       <c r="Q60" t="inlineStr"/>
       <c r="R60" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="S60" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="61">
@@ -3561,7 +3561,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>['silo', 'agricultural area with environmental restrictions', 'fallow', 'mixed cropping']</t>
+          <t>['crop yield', 'crop production', 'crop losses', 'agricultural situation', 'cereals of bread-making quality', 'agricultural region', 'cereal-growing', 'wheat', 'food cereals', 'climatic zone']</t>
         </is>
       </c>
       <c r="G61" t="inlineStr"/>
@@ -3588,10 +3588,10 @@
       <c r="P61" t="inlineStr"/>
       <c r="Q61" t="inlineStr"/>
       <c r="R61" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="S61" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
creating zero-shot classif branch
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -543,7 +543,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>['resistance of materials', 'EU energy label', 'project funding', 'clean technology', 'cultural heritage', 'EU initiative', 'energy savings', 'seismic engineering', 'advanced materials', 'building renovation']</t>
+          <t>['disaster risk reduction', 'cultural heritage', 'advanced materials', 'earthquake', 'energy efficiency', 'energy consumption']</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
@@ -566,10 +566,10 @@
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S2" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="3">
@@ -590,7 +590,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>['smart city', 'smart technology', 'smart specialisation', 'open science', 'popularising science', 'knowledge economy', 'bibliometric analysis', 'scientific publications', 'technological innovation', 'concentration of the population']</t>
+          <t>['information technology', 'smart city', 'digital technology', 'sustainable development', 'scientific research']</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -641,7 +641,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>['adaptation to climate change', 'services of general interest', 'impact of information technology', 'search and rescue', 'crisis management', 'knowledge management', 'carbon capture and storage', 'Paris Agreement on Climate Change', 'risk management', 'economic instrument for the environment']</t>
+          <t>['decision-making', 'climate change', 'innovation']</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
@@ -698,7 +698,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>['knowledge management', 'disaster prevention', 'risk assessment', 'climate change', 'risk communication', 'scientific research', 'decision-making process', 'resilience', 'transboundary cooperation', 'social dimension']</t>
+          <t>['climate change', 'disaster risk reduction', 'scientific cooperation', 'data sharing']</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
@@ -725,10 +725,10 @@
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="S5" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6">
@@ -749,7 +749,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>['waste recycling', 'municipal waste', 'circular economy', 'social labelling', 'pre-packaging', 'economic instrument for the environment', 'hazardous waste', 'hygiene product', 'environmental tax', 'product recall']</t>
+          <t>['circular economy', 'harmonisation of standards', 'waste management', 'environmental protection', 'environmental policy', 'packaging']</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
@@ -776,10 +776,10 @@
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="n">
-        <v>0.3333333333333333</v>
+        <v>0</v>
       </c>
       <c r="S6" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -800,7 +800,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>['data sharing', 'spatial data', 'data governance', 'technical standard', 'European Interoperability Framework', 'machine-readable data', 'public data', 'open data', 'satellite data', 'technical barriers to trade']</t>
+          <t>['harmonisation of standards', 'data sharing', 'EU policy', 'agricultural policy']</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
@@ -827,10 +827,10 @@
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S7" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="8">
@@ -851,7 +851,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>['aid evaluation', 'EU initiative', 'data governance', 'evaluation method', 'project evaluation', 'policy analysis', 'EU financial instrument', 'on line data service', 'multi-level governance', 'European Data Protection Board']</t>
+          <t>['EU policy', 'microeconomics', 'econometrics', 'European Commission']</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
@@ -881,7 +881,7 @@
         <v>0.3333333333333333</v>
       </c>
       <c r="S8" t="n">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="9">
@@ -903,7 +903,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>['economic instrument for the environment', 'degradation of the environment', 'quality of the environment', 'competence of the institution', 'opinion of the Commission', 'implementation of the budget', 'operation of the Institutions', 'liberalisation of the market', 'adoption of the budget', 'Institution of the Union']</t>
+          <t>['energy storage', 'regulation', 'sustainable development', 'environmental policy', 'European Commission']</t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
@@ -954,7 +954,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>['policy analysis', 'knowledge economy', 'EU study report', 'Internet of Things', 'impact of information technology', 'monitoring report', 'promotion of the European idea', 'adoption of the budget', 'liberalisation of the market', 'operation of the Institutions']</t>
+          <t>['robotics', 'artificial intelligence', 'industrial policy']</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
@@ -981,10 +981,10 @@
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
       <c r="R10" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="S10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -1005,7 +1005,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>['trade agreement (EU)', 'terms of trade', 'supply chain', 'raw material', 'value chain', 'EU strategy', 'technical barriers to trade', 'country of origin principle', 'economic governance (EU)', 'Central and Eastern European countries']</t>
+          <t>['European Union', 'trade relations', 'supply chain', 'Ukraine', 'Kazakhstan', 'Russia', 'raw material', 'international trade']</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
@@ -1032,10 +1032,10 @@
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
       <c r="R11" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="S11" t="n">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="12">
@@ -1056,7 +1056,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>['Southern neighbourhood', 'Union for the Mediterranean', 'mode of production', 'impact of information technology', 'reform of the CAP', 'economic instrument for the environment', 'sea level rise', 'concentration of the population', 'composition of the population', 'right to development']</t>
+          <t>['Tunisia', 'Egypt', 'agricultural policy', 'Algeria', 'Morocco', 'drought', 'biomass', 'Libya', 'Maghreb']</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>['smart technology', 'liberalisation of the market', 'economic instrument for the environment', 'European Interoperability Framework', 'public policy', 'energy poverty', 'smart specialisation', 'withdrawal from the market', 'interoperability', 'consumer empowerment']</t>
+          <t>['energy policy', 'European Commission', 'energy efficiency', 'smart technology']</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
@@ -1134,10 +1134,10 @@
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
       <c r="R13" t="n">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="S13" t="n">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="14">
@@ -1158,7 +1158,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>['critical infrastructure security', 'aviation security', 'common security and defence policy', 'public-private partnership', 'area of freedom', 'security and justice', 'systems interconnection', 'impact of information technology', 'Internet of Things', 'climate security', 'text and data mining']</t>
+          <t>['risk management', 'private sector', 'public safety', 'public space', 'drone']</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
@@ -1185,10 +1185,10 @@
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="S14" t="n">
-        <v>0.09090909090909091</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="15">
@@ -1209,7 +1209,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>['digital transformation', 'digital literacy', 'digital rights management', 'digital content', 'economic governance (EU)', 'economic instrument for the environment', 'inclusion in the budget', 'Institution of the Union', 'financing of the EU budget', 'competence of the institution']</t>
+          <t>['European Union', 'information technology', 'research and development', 'globalisation', 'economic analysis', 'digital technology', 'economic indicator', 'digital economy', 'technology assessment', 'digital transformation']</t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
@@ -1236,10 +1236,10 @@
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
       <c r="R15" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="S15" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="16">
@@ -1260,7 +1260,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>['crop rotation', 'mixed cropping', 'mode of production', 'Southern neighbourhood', 'European Neighbourhood and Partnership Instrument', 'Union for the Mediterranean', 'economic instrument for the environment', 'EU strategy', 'strategic partnership (EU)', 'impact of information technology']</t>
+          <t>['crop yield', 'agricultural statistics', 'agricultural policy', 'Ukraine', 'food security', 'agricultural production']</t>
         </is>
       </c>
       <c r="G16" t="inlineStr"/>
@@ -1287,10 +1287,10 @@
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
       <c r="R16" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="S16" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="17">
@@ -1311,7 +1311,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>['monitoring report', 'disaster prevention', 'disaster management', 'resilience', 'risk assessment', 'environmental monitoring', 'data collection', 'European Union', 'implementation of EU policies', 'knowledge management']</t>
+          <t>['knowledge management', 'disaster risk reduction', 'data collection', 'civil defence']</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
@@ -1338,10 +1338,10 @@
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
       <c r="R17" t="n">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="S17" t="n">
-        <v>0.2</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="18">
@@ -1362,7 +1362,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>['food contact material', 'food safety', 'food technology', 'mineral oil', 'food hygiene', 'food chain', 'food systems', 'food additive', 'food security', 'food-borne disease']</t>
+          <t>['consumer protection', 'food contamination', 'public health', 'food safety']</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
@@ -1389,10 +1389,10 @@
       <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr"/>
       <c r="R18" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="S18" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="19">
@@ -1413,7 +1413,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>['special education', 'comparative education', 'cooperation in the field of education', 'inclusion in the budget', 'intercultural competences', 'democratic competences', 'social cohesion', 'active citizenship', 'pluralism in the media', 'economic and social cohesion']</t>
+          <t>['European Union', 'teacher training']</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
@@ -1440,10 +1440,10 @@
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr"/>
       <c r="R19" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S19" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20">
@@ -1464,7 +1464,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>['routing security', 'interoperability of networks', 'internet governance', 'information technology', 'cybersecurity', 'EU Member State', 'global network', 'adoption of standards', 'network operator', 'data analysis']</t>
+          <t>['European Union', 'information technology', 'telecommunications policy', 'data protection', 'standardisation']</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
@@ -1491,10 +1491,10 @@
       <c r="P20" t="inlineStr"/>
       <c r="Q20" t="inlineStr"/>
       <c r="R20" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="S20" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1515,7 +1515,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>['critical infrastructure security', 'EU alert system', 'area of freedom', 'security and justice', 'competence of the Member States', 'operation of the Institutions', 'primacy of EU law', 'Treaty on the Functioning of the EU', 'independence of the judiciary', 'payment system', 'liberalisation of the market']</t>
+          <t>['information security', 'data protection', 'EU Member State']</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
@@ -1542,10 +1542,10 @@
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr"/>
       <c r="R21" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="S21" t="n">
-        <v>0.09090909090909091</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1566,7 +1566,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>['impact of information technology', 'degradation of the environment', 'quality of the environment', 'economic instrument for the environment', 'concentration of the population', 'composition of the population', 'Union for the Mediterranean', 'exploitation of the seas', 'freedom of the skies', 'apparatus based on the use of rays']</t>
+          <t>['humanitarian aid', 'natural disaster', 'international cooperation', 'disaster risk reduction', 'remote sensing', 'earthquake']</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
@@ -1593,10 +1593,10 @@
       <c r="P22" t="inlineStr"/>
       <c r="Q22" t="inlineStr"/>
       <c r="R22" t="n">
-        <v>0</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="S22" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="23">
@@ -1619,7 +1619,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>['mineral oil', 'food contact material', 'EU reference laboratory', 'European Union', 'EU study report', 'recommendation (EU)', 'oil refining', 'oil pollution', 'oil industry', 'edible oil']</t>
+          <t>['European Union', 'food contact material', 'mineral oil', 'food safety', 'public health']</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
@@ -1670,7 +1670,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>['research and development', 'Joint Research Centre', 'research', 'research infrastructure', 'industrial research', 'environmental research', 'Scientific and Technical Research Committee', 'European Joint Undertaking', 'Framework Programme for Research and Development', 'think tank']</t>
+          <t>['nuclear energy', 'international cooperation', 'scientific cooperation', 'research and development']</t>
         </is>
       </c>
       <c r="G24" t="inlineStr"/>
@@ -1721,7 +1721,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>['digital transformation', 'digital economy', 'economic and social cohesion', 'economic instrument for the environment', 'digital divide', 'smart city', 'Internet of Things', 'open science', 'EU macroregional policy', 'relations between the State and the regions']</t>
+          <t>['patent', 'European Union', 'regional development', 'research and development', 'international cooperation', 'United States', 'geographical distribution', 'digital technology', 'knowledge transfer', 'innovation', 'Japan']</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
@@ -1751,7 +1751,7 @@
         <v>0.2</v>
       </c>
       <c r="S25" t="n">
-        <v>0.1</v>
+        <v>0.09090909090909091</v>
       </c>
     </row>
     <row r="26">
@@ -1772,7 +1772,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>['marine litter', 'marine environment', 'environmental monitoring', 'harmonisation of legislation', 'environmental protection', 'degradation of the environment', 'exploitation of the seas', 'freedom of the seas', 'competence of the Member States', 'implementation of EU law']</t>
+          <t>['environmental monitoring', 'data collection', 'marine pollution', 'EU Member State', 'international cooperation', 'sustainable development', 'waste management', 'marine environment', 'environmental protection', 'environmental policy']</t>
         </is>
       </c>
       <c r="G26" t="inlineStr"/>
@@ -1799,10 +1799,10 @@
       <c r="P26" t="inlineStr"/>
       <c r="Q26" t="inlineStr"/>
       <c r="R26" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="S26" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="27">
@@ -1823,7 +1823,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>['plant health control', 'food security', 'technical standard', 'EU reference laboratory', 'novel food', 'food hygiene', 'EU study report', 'industrial research', 'economic instrument for the environment', 'quality control of industrial products']</t>
+          <t>['European Union', 'traceability', 'genetically modified organism', 'new technology', 'legislation', 'food safety']</t>
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
@@ -1850,10 +1850,10 @@
       <c r="P27" t="inlineStr"/>
       <c r="Q27" t="inlineStr"/>
       <c r="R27" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S27" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="28">
@@ -1874,7 +1874,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>['renewable fuel', 'water', 'water management', 'water supply', 'water treatment', 'water policy', 'testing', 'degradation of the environment', 'EU strategy', 'soft energy']</t>
+          <t>['hydrogen', 'renewable energy', 'energy technology', 'environmental protection', 'energy efficiency']</t>
         </is>
       </c>
       <c r="G28" t="inlineStr"/>
@@ -1901,10 +1901,10 @@
       <c r="P28" t="inlineStr"/>
       <c r="Q28" t="inlineStr"/>
       <c r="R28" t="n">
-        <v>0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="S28" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="29">
@@ -1925,7 +1925,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>['hazardous waste', 'waste statistics', 'waste recycling', 'waste incineration', 'economic instrument for the environment', 'environmental tax', 'public sanitation', 'Treaty on the Functioning of the EU', 'waste management', 'environmental sustainability']</t>
+          <t>['energy recovery', 'sustainable development', 'waste management', 'hazardous waste', 'industrial waste', 'environmental policy']</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
@@ -1952,10 +1952,10 @@
       <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr"/>
       <c r="R29" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="S29" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1976,7 +1976,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>['crisis management', 'disaster prevention', 'disaster preparedness', 'disaster response', 'risk assessment', 'satellite imagery', 'geographical information system', 'European Commission', 'interdisciplinary research', 'situational awareness']</t>
+          <t>['geographical information system', 'Joint Research Centre', 'crisis management', 'capacity building', 'European Commission']</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
@@ -2006,7 +2006,7 @@
         <v>0.2</v>
       </c>
       <c r="S30" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="31">
@@ -2027,7 +2027,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>['South America', 'drought', 'America', 'Latin America', 'South-South cooperation']</t>
+          <t>['natural disaster', 'heatwave', 'climate change', 'South America', 'drought', 'environmental impact']</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
@@ -2078,7 +2078,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>['quality of the environment', 'degradation of the environment', 'economic instrument for the environment', 'physico-chemical property', 'safety assessment', 'nanotechnology', 'environmental impact', 'standardisation', 'laboratory test', 'OECD']</t>
+          <t>['standardisation', 'environmental protection', 'environmental impact', 'OECD', 'nanotechnology']</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
@@ -2108,7 +2108,7 @@
         <v>0.5</v>
       </c>
       <c r="S32" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="33">
@@ -2129,7 +2129,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>['economic instrument for the environment', 'freedom of the seas', 'exploitation of the seas', 'degradation of the environment', 'quality of the environment', 'law of the sea', 'implementation of the budget', 'reform of the CAP', 'inclusion in the budget', 'relations between the State and the regions']</t>
+          <t>['international cooperation', 'climate change', 'sustainable development', 'marine environment', 'environmental protection', 'marine ecosystem', 'environmental policy', 'EU policy']</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
@@ -2180,7 +2180,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>['agricultural economics', 'common agricultural policy', 'economic accounts for agriculture', 'agro-industry', 'EU direct payments', 'trade agreement (EU)', 'redirection of production', 'economic governance (EU)', 'agricultural levy', 'EU initiative']</t>
+          <t>['public data', 'agricultural trade', 'European Union', 'data collection', 'consumption', 'agricultural statistics', 'agricultural policy', 'agricultural production']</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
@@ -2207,10 +2207,10 @@
       <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr"/>
       <c r="R34" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S34" t="n">
         <v>0.25</v>
-      </c>
-      <c r="S34" t="n">
-        <v>0.1</v>
       </c>
     </row>
     <row r="35">
@@ -2231,7 +2231,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>['economic instrument for the environment', 'liberalisation of the market', 'degradation of the environment', 'quality of the environment', 'quality control of industrial products', 'concentration of the population', 'composition of the population', 'coaching in the workplace', 'geographical distribution of the population', 'exploitation of the seas']</t>
+          <t>['heat pump', 'supply chain', 'renewable energy', 'sustainable development', 'energy policy', 'energy transition', 'energy efficiency', 'environmental impact']</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
@@ -2258,10 +2258,10 @@
       <c r="P35" t="inlineStr"/>
       <c r="Q35" t="inlineStr"/>
       <c r="R35" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S35" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="36">
@@ -2282,7 +2282,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>['management committee (EU)', 'European Maritime and Fisheries Fund', 'risk management', 'advisory committee (EU)', 'management', 'technical standard', 'environmental auditing', 'economic governance (EU)', 'economic instrument for the environment', 'technical barriers to trade']</t>
+          <t>['fishery resources', 'sustainable development', 'environmental protection', 'marine ecosystem', 'EU policy']</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
@@ -2333,7 +2333,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>['critical infrastructure security', 'industrial research', 'text and data mining', 'public policy', 'systems interconnection', 'adaptation to climate change', 'common security and defence policy', 'European Joint Undertaking', 'impact of information technology', 'services of general interest']</t>
+          <t>['natural disaster', 'terrorism', 'research and development', 'public safety', 'nuclear safety']</t>
         </is>
       </c>
       <c r="G37" t="inlineStr"/>
@@ -2360,10 +2360,10 @@
       <c r="P37" t="inlineStr"/>
       <c r="Q37" t="inlineStr"/>
       <c r="R37" t="n">
-        <v>0.3333333333333333</v>
+        <v>0</v>
       </c>
       <c r="S37" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -2384,7 +2384,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>['data sharing', 'data governance', 'anonymisation', 'personal data', 'privacy enhancing technologies', 'impact of information technology', 'cloud computing', 'machine-readable data', 'digital infrastructure supply', 'technology transfer']</t>
+          <t>['European Union', 'data sharing', 'digital technology', 'confidentiality', 'personal data', 'data protection', 'information security']</t>
         </is>
       </c>
       <c r="G38" t="inlineStr"/>
@@ -2414,7 +2414,7 @@
         <v>0.25</v>
       </c>
       <c r="S38" t="n">
-        <v>0.1</v>
+        <v>0.1428571428571428</v>
       </c>
     </row>
     <row r="39">
@@ -2435,7 +2435,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>['European Union', 'drought', 'Northern Europe', 'Southern Europe', 'Europe', 'European Union Solidarity Fund', 'economic instrument for the environment', 'member country', 'adverse climatic event', 'seasonal forecast']</t>
+          <t>['European Union', 'natural disaster', 'climate change', 'drought', 'environmental impact', 'meteorology', 'regional disparity']</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
@@ -2462,10 +2462,10 @@
       <c r="P39" t="inlineStr"/>
       <c r="Q39" t="inlineStr"/>
       <c r="R39" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="S39" t="n">
-        <v>0.1</v>
+        <v>0.2857142857142857</v>
       </c>
     </row>
     <row r="40">
@@ -2486,7 +2486,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>['reduction of gas emissions', 'carbon neutrality', 'emission trading', 'emission allowance', 'clean development mechanism', 'land use', 'Paris Agreement on Climate Change', 'Kyoto Protocol', 'carbon capture and storage', 'EU Emissions Trading Scheme']</t>
+          <t>['international agreement', 'global warming', 'climate change', 'sustainable development', 'greenhouse gas', 'environmental policy']</t>
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
@@ -2513,10 +2513,10 @@
       <c r="P40" t="inlineStr"/>
       <c r="Q40" t="inlineStr"/>
       <c r="R40" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="S40" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -2537,7 +2537,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>['economic instrument for the environment', 'degradation of the environment', 'quality of the environment', 'Health Emergency Preparedness and Response Authority', 'circular economy', 'public health', 'epidemiology', 'environmental risk', 'resilience of the economy', 'social inequality']</t>
+          <t>['circular economy', 'epidemiology', 'pollution', 'climate change', 'social inequality', 'supply chain', 'crisis management', 'public health', 'EU policy']</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
@@ -2564,10 +2564,10 @@
       <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr"/>
       <c r="R41" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="S41" t="n">
-        <v>0.1</v>
+        <v>0.2222222222222222</v>
       </c>
     </row>
     <row r="42">
@@ -2588,7 +2588,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>['load', 'damage', 'assessment', 'evaluation method', 'critical infrastructure security', 'disaster risk reduction', 'war damage', 'technology assessment', 'industrial structures', 'protection of communications']</t>
+          <t>['disaster risk reduction', 'civil engineering']</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
@@ -2639,7 +2639,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>['paints and varnishes', 'EU study report', 'economic instrument for the environment', 'recommendation (EU)', 'EU activity', 'expert group (EU)', 'economic and social cohesion']</t>
+          <t>['sustainable development', 'environmental protection', 'product safety', 'paints and varnishes', 'European Commission']</t>
         </is>
       </c>
       <c r="G43" t="inlineStr"/>
@@ -2690,7 +2690,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>['alternative investment', 'carbon neutrality', 'sustainable finance', 'gross domestic product', 'EU financial instrument', 'data science', 'data sharing', 'public data', 'carbon capture and storage', 'open data']</t>
+          <t>['Eurostat', 'input-output analysis', 'EU Member State', 'macroeconomics', 'sustainable development', 'investment', 'energy transition', 'environmental policy']</t>
         </is>
       </c>
       <c r="G44" t="inlineStr"/>
@@ -2717,10 +2717,10 @@
       <c r="P44" t="inlineStr"/>
       <c r="Q44" t="inlineStr"/>
       <c r="R44" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="S44" t="n">
-        <v>0</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="45">
@@ -2741,7 +2741,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>['disruptive technology', 'quantum technology', 'astronautics', 'foresight', 'EU study report', 'dual-use technology', 'common security and defence policy', 'EU strategy', 'strategic partnership (EU)', 'European Union']</t>
+          <t>['European Union', 'space technology', 'disruptive technology', 'photonics', 'nuclear energy', 'space research', 'cryptography']</t>
         </is>
       </c>
       <c r="G45" t="inlineStr"/>
@@ -2768,10 +2768,10 @@
       <c r="P45" t="inlineStr"/>
       <c r="Q45" t="inlineStr"/>
       <c r="R45" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S45" t="n">
-        <v>0</v>
+        <v>0.1428571428571428</v>
       </c>
     </row>
     <row r="46">
@@ -2792,7 +2792,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>['innovation', 'research infrastructure', 'open innovation', 'knowledge economy', 'EU study report', 'value chain', 'economic geography', 'economic value', 'services of general interest', 'impact of information technology']</t>
+          <t>['public policy', 'research and development', 'policymaking', 'investment', 'technology transfer', 'economic policy', 'knowledge transfer']</t>
         </is>
       </c>
       <c r="G46" t="inlineStr"/>
@@ -2819,10 +2819,10 @@
       <c r="P46" t="inlineStr"/>
       <c r="Q46" t="inlineStr"/>
       <c r="R46" t="n">
-        <v>0.3333333333333333</v>
+        <v>0</v>
       </c>
       <c r="S46" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -2843,7 +2843,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>['forced migration', 'migration', 'environmental risk prevention', 'spatial data', 'public data', 'data science', 'environmental cooperation', 'open data', 'satellite data', 'environmental conditions']</t>
+          <t>['migration', 'climate change', 'disaster risk reduction', 'environmental impact', 'migration policy']</t>
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
@@ -2894,7 +2894,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>['land use', 'public-private partnership', 'emission trading', 'pollution from land-based sources', 'economic instrument for the environment', 'Kyoto Protocol', 'reduction of gas emissions', 'EU study report', 'public goods', 'economic governance (EU)']</t>
+          <t>['environmental monitoring', 'land use', 'climate change', 'public-private partnership', 'greenhouse gas', 'environmental policy']</t>
         </is>
       </c>
       <c r="G48" t="inlineStr"/>
@@ -2921,10 +2921,10 @@
       <c r="P48" t="inlineStr"/>
       <c r="Q48" t="inlineStr"/>
       <c r="R48" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="S48" t="n">
         <v>0.5</v>
-      </c>
-      <c r="S48" t="n">
-        <v>0.2</v>
       </c>
     </row>
     <row r="49">
@@ -2945,7 +2945,7 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>['renewable fuel', 'substitute fuel', 'energy market', 'clean technology', 'energy transition', 'solar energy', 'regulation (EU)', 'ecodesign', 'technology transfer', 'intermediate technology']</t>
+          <t>['renewable energy', 'sustainable development', 'energy policy', 'energy transition', 'solar energy']</t>
         </is>
       </c>
       <c r="G49" t="inlineStr"/>
@@ -2972,10 +2972,10 @@
       <c r="P49" t="inlineStr"/>
       <c r="Q49" t="inlineStr"/>
       <c r="R49" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S49" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="50">
@@ -2996,7 +2996,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>['aid evaluation', 'control of State aid', 'financial stability', 'EU initiative', 'economic instrument for the environment', 'Treaty on the Functioning of the EU', 'relations between the State and the regions', 'balance of payments assistance', 'financing of the EU budget', 'EU strategy']</t>
+          <t>['Poland', 'Spain', 'Italy', 'economic recovery', 'crisis management', 'small and medium-sized enterprises', 'public health']</t>
         </is>
       </c>
       <c r="G50" t="inlineStr"/>
@@ -3048,7 +3048,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>['forest', 'carbon capture and storage', 'nature restoration', 'EU strategy', 'forest certification', 'open data', 'text and data mining', 'economic instrument for the environment', 'public data', 'management information system']</t>
+          <t>['data collection', 'remote sensing', 'renewable energy', 'sustainable development', 'biodiversity', 'environmental policy']</t>
         </is>
       </c>
       <c r="G51" t="inlineStr"/>
@@ -3099,7 +3099,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>['competence of the Member States', 'business-to-consumer', 'liberalisation of the market', 'quality of the environment', 'economic instrument for the environment', 'consumer organisations', 'artificial intelligence', 'single market', 'monitoring system', 'Member States']</t>
+          <t>['European Union', 'consumer protection', 'mobile application', 'artificial intelligence', 'single market', 'food industry']</t>
         </is>
       </c>
       <c r="G52" t="inlineStr"/>
@@ -3150,7 +3150,7 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>['biodiversity', 'land use', 'agroforestry', 'cocoa', 'land governance', 'nature restoration', 'land reform', 'food systems', 'pollution from land-based sources', 'ecological tourism']</t>
+          <t>['cultivation system', 'land use', 'agroforestry', 'cocoa', 'biodiversity', 'comparative analysis', 'environmental impact', 'sustainable agriculture', 'protected area']</t>
         </is>
       </c>
       <c r="G53" t="inlineStr"/>
@@ -3180,7 +3180,7 @@
         <v>0.3333333333333333</v>
       </c>
       <c r="S53" t="n">
-        <v>0.2</v>
+        <v>0.2222222222222222</v>
       </c>
     </row>
     <row r="54">
@@ -3201,7 +3201,7 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>['common fisheries policy', 'Protocol (EU)', 'fisheries policy', 'European Maritime and Fisheries Fund', 'exploitation of the seas', 'economic instrument for the environment', 'policy analysis', 'Treaty on the Functioning of the EU', 'EU policy - national policy', 'degradation of the environment']</t>
+          <t>['environmental monitoring', 'data collection', 'sustainable development', 'fishery management', 'fisheries policy']</t>
         </is>
       </c>
       <c r="G54" t="inlineStr"/>
@@ -3254,7 +3254,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>['Paris Agreement on Climate Change', 'energy transition', 'reduction of gas emissions', 'adaptation to climate change', 'economic instrument for the environment', 'energy market', 'sustainable finance', 'energy audit', 'climate security', 'carbon capture and storage']</t>
+          <t>['energy supply', 'climate change', 'energy production', 'sustainable development', 'energy policy', 'investment', 'energy demand', 'energy transition']</t>
         </is>
       </c>
       <c r="G55" t="inlineStr"/>
@@ -3281,10 +3281,10 @@
       <c r="P55" t="inlineStr"/>
       <c r="Q55" t="inlineStr"/>
       <c r="R55" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S55" t="n">
-        <v>0</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="56">
@@ -3305,7 +3305,7 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>['degradation of the environment', 'quality of the environment', 'concentration of the population', 'composition of the population', 'economic instrument for the environment', 'evacuation of the population']</t>
+          <t>['natural disaster', 'heatwave', 'climate change', 'South America', 'drought', 'environmental impact']</t>
         </is>
       </c>
       <c r="G56" t="inlineStr"/>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>['economic instrument for the environment', 'degradation of the environment', 'quality of the environment', 'Internet of Things', 'liberalisation of the market', 'telecommunications', 'sustainability', 'environmental impact', 'digital technology', 'energy efficiency']</t>
+          <t>['telecommunications', 'environmental indicator', 'digital technology', 'energy policy', 'code of conduct', 'environmental impact']</t>
         </is>
       </c>
       <c r="G57" t="inlineStr"/>
@@ -3408,7 +3408,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>['climate change', 'climate change policy', 'adaptation to climate change', 'carbon', 'carbon neutrality', 'carbon capture and storage', 'reduction of gas emissions', 'forest', 'economic instrument for the environment', 'final consumption']</t>
+          <t>['climate change', 'natural resources', 'sustainable development', 'environmental impact']</t>
         </is>
       </c>
       <c r="G58" t="inlineStr"/>
@@ -3435,10 +3435,10 @@
       <c r="P58" t="inlineStr"/>
       <c r="Q58" t="inlineStr"/>
       <c r="R58" t="n">
-        <v>0.1666666666666667</v>
+        <v>0</v>
       </c>
       <c r="S58" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -3459,7 +3459,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>['economic instrument for the environment', 'quality control of industrial products', 'text and data mining', 'systems interconnection', 'degradation of the environment', 'liberalisation of the market', 'impact of information technology', 'inclusion in the budget', 'right to development', 'exploitation of the seas']</t>
+          <t>['data sharing', 'international cooperation', 'decision-making', 'supply chain', 'new technology', 'sustainable development', 'database', 'industrial policy', 'scientific cooperation', 'environmental impact']</t>
         </is>
       </c>
       <c r="G59" t="inlineStr"/>
@@ -3486,10 +3486,10 @@
       <c r="P59" t="inlineStr"/>
       <c r="Q59" t="inlineStr"/>
       <c r="R59" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="S59" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="60">
@@ -3510,7 +3510,7 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>['crop yield', 'European Neighbourhood and Partnership Instrument', 'Southern neighbourhood', 'marketing year', 'fallow', 'crop rotation', 'mixed cropping', 'heatwave', 'economic accounts for agriculture', 'Union for the Mediterranean']</t>
+          <t>['crop yield', 'Türkiye', 'agricultural production']</t>
         </is>
       </c>
       <c r="G60" t="inlineStr"/>
@@ -3561,7 +3561,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>['European Neighbourhood and Partnership Instrument', 'European Union', 'Southern neighbourhood', 'Russia', 'crop monitoring', 'winter cereals', 'spring cereals', 'grain maize', 'unfavourable weather', 'agricultural production.']</t>
+          <t>['crop yield', 'Russia', 'agricultural policy', 'agricultural production']</t>
         </is>
       </c>
       <c r="G61" t="inlineStr"/>

</xml_diff>

<commit_message>
create iterative approach branch
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -543,7 +543,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>['resistance of materials', 'energy audit', 'building performance']</t>
+          <t>['energy efficiency', 'seismic monitoring', 'building safety', 'cultural heritage', 'advanced materials', 'energy consumption', 'heritage protection', 'natural hazard', 'building performance', 'innovation']</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
@@ -590,7 +590,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>['smart city', 'Internet of Things', 'smart technology', 'prospective technological studies', 'smart specialisation']</t>
+          <t>['smart city', 'urban infrastructure', 'sustainable development', 'information technology', 'technological process', 'urban economy', 'urbanisation', 'research', 'innovation', 'urban sociology']</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -641,7 +641,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>['adaptation to climate change', 'climate security', 'natural disaster', 'crisis management', 'geographical information system']</t>
+          <t>['satellite data', 'climate change', 'adaptation to climate change', 'geographical information system', 'spatial data', 'remote sensing', 'risk management', 'disaster risk reduction', 'environmental monitoring', 'crisis management']</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
@@ -668,10 +668,10 @@
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr"/>
       <c r="R4" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S4" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="5">
@@ -698,7 +698,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>['adaptation to climate change', 'community resilience', 'citizen science', 'natural disaster', 'popularising science']</t>
+          <t>['organisation of research', 'data sharing', 'research policy', 'climate change', 'adaptation to climate change', 'risk management', 'disaster risk reduction', 'cross-border cooperation', 'scientific cooperation', 'natural hazard']</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
@@ -725,10 +725,10 @@
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="n">
-        <v>0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="S5" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="6">
@@ -749,7 +749,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>['municipal waste', 'waste recycling', 'circular economy']</t>
+          <t>['waste management', 'packaging', 'consumer information', 'waste recycling', 'environmental protection', 'circular economy', 'labelling', 'recycled product', 'domestic waste', 'environmental impact']</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
@@ -776,10 +776,10 @@
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="S6" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="7">
@@ -800,7 +800,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>['data sharing', 'European Interoperability Framework', 'systems interconnection', 'data governance']</t>
+          <t>['harmonisation of standards', 'information system', 'data sharing', 'geographical information system', 'European Interoperability Framework', 'spatial data', 'systems interconnection', 'standardisation', 'exchange of information', 'data collection']</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
@@ -827,10 +827,10 @@
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S7" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="8">
@@ -851,7 +851,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>['EU study report', 'EU reference laboratory']</t>
+          <t>['European Commission', 'EU policy', 'evaluation method', 'econometrics', 'microeconomics', 'economic analysis', 'data processing', 'evidence', 'policy analysis', 'impact study']</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
@@ -878,10 +878,10 @@
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
       <c r="R8" t="n">
-        <v>0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="S8" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="9">
@@ -903,7 +903,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>['quality standard', 'ecodesign']</t>
+          <t>['Joint Research Centre', 'EU environmental policy', 'sustainable development', 'consultation procedure', 'delegated legislation', 'public consultation', 'environmental protection', 'energy storage', 'performance measurement', 'technical specification']</t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
@@ -954,7 +954,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>['EU study report', 'EU policy - national policy', 'prospective technological studies']</t>
+          <t>['robotisation', 'diffusion of innovations', 'industrial policy', 'economic development', 'automation', 'advanced technology industry', 'industrial robot', 'robotics', 'innovation', 'technological change']</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
@@ -981,10 +981,10 @@
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
       <c r="R10" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="S10" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="11">
@@ -1005,7 +1005,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>['supply chain', 'raw material', 'terms of trade', 'EU market']</t>
+          <t>['Kazakhstan', 'raw material', 'international trade', 'trade relations', 'trade statistics', 'supply chain', 'security of supply', 'import (EU)', 'export (EU)', 'geopolitical impact']</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
@@ -1032,10 +1032,10 @@
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
       <c r="R11" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="S11" t="n">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="12">
@@ -1056,7 +1056,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>['crop rotation', 'agricultural economics', 'precision agriculture']</t>
+          <t>['cereals', 'drought', 'crop yield', 'Maghreb', 'North Africa', 'agricultural region', 'agricultural productivity', 'Tunisia', 'Libya', 'Morocco']</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
@@ -1083,10 +1083,10 @@
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr"/>
       <c r="R12" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="S12" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="13">
@@ -1107,7 +1107,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>['smart technology', 'European Interoperability Framework', 'systems interconnection']</t>
+          <t>['household electrical appliance', 'harmonisation of standards', 'consumer', 'energy efficiency', 'energy grid', 'systems interconnection', 'European standard', 'energy consumption', 'energy policy', 'standardisation']</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
@@ -1137,7 +1137,7 @@
         <v>0.25</v>
       </c>
       <c r="S13" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="14">
@@ -1158,7 +1158,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>['aviation security', 'critical infrastructure security', 'drone']</t>
+          <t>['critical infrastructure security', 'public safety', 'drone', 'risk management', 'public space', 'surveillance', 'accident prevention', 'protective equipment', 'engineering structure', 'security services']</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
@@ -1185,10 +1185,10 @@
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="n">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="S14" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="15">
@@ -1209,7 +1209,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>['digital transformation', 'impact of information technology', 'economic intelligence', 'economic governance (EU)']</t>
+          <t>['digital transformation', 'digital economy', 'information technology', 'innovation', 'research and development', 'economic statistics', 'technological change', 'globalisation', 'policy analysis', 'prospective technological studies']</t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
@@ -1239,7 +1239,7 @@
         <v>0.25</v>
       </c>
       <c r="S15" t="n">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="16">
@@ -1260,7 +1260,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>['mixed cropping', 'crop rotation', 'adaptation to climate change', 'marketing year']</t>
+          <t>['Ukraine', 'cereals', 'crop production', 'crop yield', 'agricultural production', 'agricultural situation', 'climatic zone', 'bad weather', 'destruction of crops', 'agricultural productivity']</t>
         </is>
       </c>
       <c r="G16" t="inlineStr"/>
@@ -1287,10 +1287,10 @@
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
       <c r="R16" t="n">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="S16" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="17">
@@ -1311,7 +1311,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>['community resilience', 'monitoring report', 'risk management']</t>
+          <t>['disaster risk reduction', 'risk management', 'environmental indicator', 'data collection', 'information system', 'environmental monitoring', 'crisis management', 'community resilience', 'cartography', 'database']</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
@@ -1338,10 +1338,10 @@
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
       <c r="R17" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="S17" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="18">
@@ -1362,7 +1362,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>['food contact material', 'food safety']</t>
+          <t>['food safety', 'mineral oil', 'food contact material', 'sampling', 'analytical chemistry', 'food contamination', 'food inspection', 'chemical pollution', 'recommendation (EU)', 'hydrocarbon']</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
@@ -1389,10 +1389,10 @@
       <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr"/>
       <c r="R18" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="S18" t="n">
         <v>0.2</v>
-      </c>
-      <c r="S18" t="n">
-        <v>0.5</v>
       </c>
     </row>
     <row r="19">
@@ -1413,7 +1413,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>['basic education', 'special education', 'economic and social cohesion']</t>
+          <t>['access to education', 'inclusive education', 'teacher training', 'education policy', 'social integration', 'citizenship', 'cultural identity', 'teaching method', 'educational reform', 'social development']</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
@@ -1440,10 +1440,10 @@
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr"/>
       <c r="R19" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S19" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="20">
@@ -1464,7 +1464,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>['critical infrastructure security']</t>
+          <t>['Internet', 'information security', 'critical infrastructure security', 'telecommunications industry', 'systems interconnection', 'European standard', 'international standard', 'compliance audit', 'information network', 'data governance']</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
@@ -1491,10 +1491,10 @@
       <c r="P20" t="inlineStr"/>
       <c r="Q20" t="inlineStr"/>
       <c r="R20" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="S20" t="n">
         <v>0.2</v>
-      </c>
-      <c r="S20" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -1515,7 +1515,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>['critical infrastructure security', 'European Interoperability Framework']</t>
+          <t>['information security', 'critical infrastructure security', 'Internet', 'computer network', 'systems interconnection', 'information technology', 'digital technology', 'EU Member State', 'globalisation', 'Internet address']</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
@@ -1542,10 +1542,10 @@
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr"/>
       <c r="R21" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="S21" t="n">
         <v>0.2</v>
-      </c>
-      <c r="S21" t="n">
-        <v>0.5</v>
       </c>
     </row>
     <row r="22">
@@ -1566,7 +1566,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>['international humanitarian law', 'aid evaluation', 'European Union Solidarity Fund', 'search and rescue']</t>
+          <t>['earthquake', 'critical infrastructure security', 'humanitarian crisis', 'natural disaster', 'disaster risk reduction', 'remote sensing', 'international aid', 'Türkiye', 'Syria', 'humanitarian aid']</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
@@ -1593,10 +1593,10 @@
       <c r="P22" t="inlineStr"/>
       <c r="Q22" t="inlineStr"/>
       <c r="R22" t="n">
-        <v>0</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="S22" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="23">
@@ -1619,7 +1619,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>['food contact material', 'EU reference laboratory', 'food safety', 'recommendation (EU)']</t>
+          <t>['food safety', 'vegetable oil', 'mineral oil', 'food contact material', 'European Commission', 'EU reference laboratory', 'food inspection', 'food contamination', 'testing', 'foodstuffs legislation']</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
@@ -1646,10 +1646,10 @@
       <c r="P23" t="inlineStr"/>
       <c r="Q23" t="inlineStr"/>
       <c r="R23" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="S23" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="24">
@@ -1670,7 +1670,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>['research infrastructure', 'European Joint Undertaking']</t>
+          <t>['Joint Research Centre', 'organisation of research', 'research and development', 'research body', 'nuclear research', 'scientific cooperation', 'international cooperation', 'association', 'European association', 'research programme']</t>
         </is>
       </c>
       <c r="G24" t="inlineStr"/>
@@ -1697,10 +1697,10 @@
       <c r="P24" t="inlineStr"/>
       <c r="Q24" t="inlineStr"/>
       <c r="R24" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="S24" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="25">
@@ -1721,7 +1721,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>['digital economy', 'digital transformation', 'clean technology', 'prospective technological studies', 'region-EU relationship']</t>
+          <t>['green technology', 'digital technology', 'patents', 'regional development', 'geographical distribution', 'research and development', 'innovation', 'European Union', 'Germany', 'United States']</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
@@ -1751,7 +1751,7 @@
         <v>0.2</v>
       </c>
       <c r="S25" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="26">
@@ -1772,7 +1772,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>['monitoring report', 'pollution from land-based sources', 'integrated maritime policy', 'national competent authority']</t>
+          <t>['marine pollution', 'marine environment', 'environmental monitoring', 'waste management', 'plastic waste', 'coastal pollution', 'data collection', 'harmonisation of standards', 'environmental protection', 'marine ecosystem']</t>
         </is>
       </c>
       <c r="G26" t="inlineStr"/>
@@ -1799,10 +1799,10 @@
       <c r="P26" t="inlineStr"/>
       <c r="Q26" t="inlineStr"/>
       <c r="R26" t="n">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="S26" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="27">
@@ -1823,7 +1823,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>['EU reference laboratory', 'quality control of industrial products', 'production control']</t>
+          <t>['genetically modified organism', 'traceability', 'genetic engineering', 'biotechnology', 'food safety', 'analytical chemistry', 'legislation', 'European Union', 'plant health product', 'new technology']</t>
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
@@ -1850,10 +1850,10 @@
       <c r="P27" t="inlineStr"/>
       <c r="Q27" t="inlineStr"/>
       <c r="R27" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S27" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="28">
@@ -1874,7 +1874,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>['renewable fuel', 'soft energy', 'water resources']</t>
+          <t>['hydrogen production', 'renewable energy', 'clean technology', 'energy technology', 'electrochemistry', 'solar energy', 'wind energy', 'energy research', 'hydrogen', 'energy conversion']</t>
         </is>
       </c>
       <c r="G28" t="inlineStr"/>
@@ -1901,10 +1901,10 @@
       <c r="P28" t="inlineStr"/>
       <c r="Q28" t="inlineStr"/>
       <c r="R28" t="n">
-        <v>0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="S28" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="29">
@@ -1925,7 +1925,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>['waste statistics', 'hazardous waste', 'waste recycling', 'circular economy']</t>
+          <t>['waste management', 'waste recycling', 'hazardous waste', 'used oil', 'lubricants', 'energy recovery', 'waste incineration', 'EU law', 'environmental protection', 'EC Directive']</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
@@ -1952,10 +1952,10 @@
       <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr"/>
       <c r="R29" t="n">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="S29" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="30">
@@ -1976,7 +1976,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>['crisis management', 'risk management', 'disaster risk reduction']</t>
+          <t>['Joint Research Centre', 'satellite data', 'geographical information system', 'cartography', 'natural hazard', 'disaster risk reduction', 'crisis management', 'risk management', 'remote sensing', 'damage.']</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
@@ -2006,7 +2006,7 @@
         <v>0.2</v>
       </c>
       <c r="S30" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="31">
@@ -2027,7 +2027,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>['natural disaster', 'meteorology', 'climate security', 'adaptation to climate change', 'heatwave']</t>
+          <t>['climate change', 'drought', 'heatwave', 'desertification', 'natural hazard', 'South America', 'arid zone', 'atmospheric conditions', 'global warming', 'meteorology']</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
@@ -2078,7 +2078,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>['environmental standard', 'resistance of materials', 'EU reference laboratory', 'dangerous substance']</t>
+          <t>['environmental research', 'harmonisation of standards', 'materials technology', 'nanotechnology', 'evaluation method', 'toxic substance', 'standard', 'OECD', 'testing', 'environmental protection']</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
@@ -2105,10 +2105,10 @@
       <c r="P32" t="inlineStr"/>
       <c r="Q32" t="inlineStr"/>
       <c r="R32" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S32" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="33">
@@ -2129,7 +2129,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>['European Maritime and Fisheries Fund', 'EU strategy', 'adaptation to climate change', 'EU initiative']</t>
+          <t>['marine environment', 'marine ecosystem', 'EU environmental policy', 'directive (EU)', 'climate change', 'environmental indicator', 'socioeconomic conditions', 'international cooperation', 'environmental policy', 'impact study']</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
@@ -2156,10 +2156,10 @@
       <c r="P33" t="inlineStr"/>
       <c r="Q33" t="inlineStr"/>
       <c r="R33" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="S33" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="34">
@@ -2180,7 +2180,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>['agricultural economics', 'economic accounts for agriculture', 'common agricultural policy']</t>
+          <t>['agricultural statistics', 'agricultural production', 'agricultural trade', 'data sharing', 'public data', 'economic statistics', 'trade statistics', 'agricultural market', 'EU Member State', 'data collection']</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
@@ -2207,10 +2207,10 @@
       <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr"/>
       <c r="R34" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="S34" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="35">
@@ -2231,7 +2231,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>['reduction of gas emissions', 'energy market', 'energy poverty', 'building performance']</t>
+          <t>['heat pump', 'energy grid', 'energy transition', 'energy efficiency', 'supply chain', 'environmental impact', 'heating', 'energy consumption', 'sustainable development', 'aid to disadvantaged groups']</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
@@ -2258,10 +2258,10 @@
       <c r="P35" t="inlineStr"/>
       <c r="Q35" t="inlineStr"/>
       <c r="R35" t="n">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="S35" t="n">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="36">
@@ -2282,7 +2282,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>['EU strategy', 'EU initiative']</t>
+          <t>['EU policy', 'conservation of fish stocks', 'fishery management', 'fishing regulations', 'sustainable fisheries', 'marine environment', 'fisheries policy', 'common fisheries policy', 'fishery resources', 'marine ecosystem']</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
@@ -2309,10 +2309,10 @@
       <c r="P36" t="inlineStr"/>
       <c r="Q36" t="inlineStr"/>
       <c r="R36" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S36" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="37">
@@ -2333,7 +2333,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>['European Union Solidarity Fund', 'European Stability Mechanism']</t>
+          <t>['computer', 'data processing', 'industrial hazard', 'Joint Research Centre', 'scientific report', 'critical infrastructure security', 'nuclear technology', 'natural hazard', 'simulation', 'public safety']</t>
         </is>
       </c>
       <c r="G37" t="inlineStr"/>
@@ -2360,10 +2360,10 @@
       <c r="P37" t="inlineStr"/>
       <c r="Q37" t="inlineStr"/>
       <c r="R37" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="S37" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="38">
@@ -2384,7 +2384,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>['anonymisation', 'data sharing', 'data governance', 'impact of information technology']</t>
+          <t>['protection of privacy', 'data sharing', 'data protection', 'anonymisation', 'confidentiality', 'personal data', 'information security', 'big data', 'digital technology', 'innovation']</t>
         </is>
       </c>
       <c r="G38" t="inlineStr"/>
@@ -2411,10 +2411,10 @@
       <c r="P38" t="inlineStr"/>
       <c r="Q38" t="inlineStr"/>
       <c r="R38" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S38" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="39">
@@ -2435,7 +2435,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>['European Union Solidarity Fund', 'EU macroregional policy']</t>
+          <t>['drought', 'climate change', 'water management', 'natural hazard', 'adaptation to climate change', 'water resources', 'meteorology', 'European Commission', 'Northern Europe', 'Southern Europe']</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
@@ -2462,10 +2462,10 @@
       <c r="P39" t="inlineStr"/>
       <c r="Q39" t="inlineStr"/>
       <c r="R39" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="S39" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="40">
@@ -2486,7 +2486,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>['reduction of gas emissions', 'Paris Agreement on Climate Change']</t>
+          <t>['greenhouse gas', 'climate change', 'environmental statistics', 'reduction of gas emissions', 'environmental monitoring', 'global warming', 'environmental research', 'international agreement', 'climate change policy', 'environmental protection']</t>
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
@@ -2513,10 +2513,10 @@
       <c r="P40" t="inlineStr"/>
       <c r="Q40" t="inlineStr"/>
       <c r="R40" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="S40" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -2537,7 +2537,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>['adaptation to climate change', 'Health Emergency Preparedness and Response Authority', 'European Health Union']</t>
+          <t>['climate change', 'circular economy', 'epidemiology', 'disease prevention', 'social inequality', 'environmental monitoring', 'pollution', 'public health', 'nanotechnology', 'sustainable development']</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
@@ -2564,10 +2564,10 @@
       <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr"/>
       <c r="R41" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="S41" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="42">
@@ -2588,7 +2588,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>['critical infrastructure security', 'community resilience']</t>
+          <t>['engineering structure', 'safety device', 'industrial hazard', 'building safety', 'civil engineering', 'assessment', 'disaster risk reduction', 'explosive', 'hazard science', 'risk management']</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
@@ -2615,10 +2615,10 @@
       <c r="P42" t="inlineStr"/>
       <c r="Q42" t="inlineStr"/>
       <c r="R42" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S42" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="43">
@@ -2639,7 +2639,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>['EU study report', 'recommendation (EU)']</t>
+          <t>['scientific report', 'EU environmental policy', 'European Commission', 'environmental protection', 'dangerous substance', 'eco-label', 'paints and varnishes', 'derogation from EU law', 'environmental standard', 'hazardous waste']</t>
         </is>
       </c>
       <c r="G43" t="inlineStr"/>
@@ -2690,7 +2690,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>['carbon neutrality', 'sustainable finance', 'macroeconomics']</t>
+          <t>['investment', 'economic model', 'sustainable development', 'EU statistics', 'carbon neutrality', 'energy transition', 'input-output analysis', 'economic sector', 'energy technology', 'environmental economics']</t>
         </is>
       </c>
       <c r="G44" t="inlineStr"/>
@@ -2717,10 +2717,10 @@
       <c r="P44" t="inlineStr"/>
       <c r="Q44" t="inlineStr"/>
       <c r="R44" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="S44" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="45">
@@ -2741,7 +2741,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>['disruptive technology', 'quantum technology', 'EU strategy']</t>
+          <t>['disruptive technology', 'nuclear technology', 'space technology', 'foresight', 'quantum technology', 'photonics', 'strategic autonomy', 'space research', 'innovation', 'advanced technology industry']</t>
         </is>
       </c>
       <c r="G45" t="inlineStr"/>
@@ -2768,10 +2768,10 @@
       <c r="P45" t="inlineStr"/>
       <c r="Q45" t="inlineStr"/>
       <c r="R45" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="S45" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="46">
@@ -2792,7 +2792,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>['innovation', 'research infrastructure', 'knowledge economy', 'smart specialisation']</t>
+          <t>['organisation of research', 'diffusion of innovations', 'public-private partnership', 'applied research', 'knowledge economy', 'knowledge transfer', 'innovation', 'research policy', 'technology transfer', 'regional development']</t>
         </is>
       </c>
       <c r="G46" t="inlineStr"/>
@@ -2819,10 +2819,10 @@
       <c r="P46" t="inlineStr"/>
       <c r="Q46" t="inlineStr"/>
       <c r="R46" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="S46" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="47">
@@ -2843,7 +2843,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>['forced migration', 'spatial data', 'adaptation to climate change', 'natural disaster']</t>
+          <t>['migration', 'environmental research', 'natural disaster', 'social survey', 'migration statistics', 'environmental impact', 'geographical mobility', 'internally displaced person', 'migratory movement', 'disaster risk reduction']</t>
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
@@ -2870,10 +2870,10 @@
       <c r="P47" t="inlineStr"/>
       <c r="Q47" t="inlineStr"/>
       <c r="R47" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="S47" t="n">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="48">
@@ -2894,7 +2894,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>['emission trading', 'land use', 'Kyoto Protocol', 'economic instrument for the environment']</t>
+          <t>['EU Emissions Trading Scheme', 'land use', 'greenhouse gas', 'climate change', 'reduction of gas emissions', 'environmental policy', 'EU environmental policy', 'emission trading', 'environmental protection', 'climate change policy']</t>
         </is>
       </c>
       <c r="G48" t="inlineStr"/>
@@ -2921,10 +2921,10 @@
       <c r="P48" t="inlineStr"/>
       <c r="Q48" t="inlineStr"/>
       <c r="R48" t="n">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="S48" t="n">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="49">
@@ -2945,7 +2945,7 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>['renewable fuel', 'substitute fuel']</t>
+          <t>['solar energy', 'renewable energy', 'energy technology', 'energy transition', 'carbon neutrality', 'renewable fuel', 'energy production', 'energy resources', 'sustainable development', 'reduction of gas emissions']</t>
         </is>
       </c>
       <c r="G49" t="inlineStr"/>
@@ -2972,10 +2972,10 @@
       <c r="P49" t="inlineStr"/>
       <c r="Q49" t="inlineStr"/>
       <c r="R49" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S49" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="50">
@@ -2996,7 +2996,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>['financial stability', 'EU financing', 'EU financial instrument']</t>
+          <t>['economic stabilisation', 'economic aid', 'short-term financing', 'financial market', 'company in difficulties', 'small and medium-sized enterprises', 'State aid', 'coronavirus disease', 'liquidity control', 'impact study']</t>
         </is>
       </c>
       <c r="G50" t="inlineStr"/>
@@ -3023,10 +3023,10 @@
       <c r="P50" t="inlineStr"/>
       <c r="Q50" t="inlineStr"/>
       <c r="R50" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="S50" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="51">
@@ -3048,7 +3048,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>['nature restoration', 'carbon capture and storage', 'EU strategy', 'remote sensing']</t>
+          <t>['EU policy', 'EU environmental policy', 'biodiversity', 'climate change policy', 'forestry policy', 'sustainable forest management', 'carbon', 'data collection', 'remote sensing', 'forestry research']</t>
         </is>
       </c>
       <c r="G51" t="inlineStr"/>
@@ -3075,10 +3075,10 @@
       <c r="P51" t="inlineStr"/>
       <c r="Q51" t="inlineStr"/>
       <c r="R51" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="S51" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="52">
@@ -3099,7 +3099,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>['business-to-consumer', 'smart technology', 'quality control of industrial products', 'multilateral surveillance']</t>
+          <t>['consumer protection', 'consumer policy', 'single market', 'artificial intelligence', 'mobile application', 'public awareness campaign', 'product quality', 'feasibility study', 'consumer behaviour', 'food industry']</t>
         </is>
       </c>
       <c r="G52" t="inlineStr"/>
@@ -3150,7 +3150,7 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>['biodiversity', 'agroforestry', 'land use', 'plantation']</t>
+          <t>['biodiversity', 'agroforestry', 'land use', 'cultivation system', 'environmental impact', 'comparative analysis', 'protected area', 'agricultural land', 'sustainable agriculture', 'terrestrial ecosystem']</t>
         </is>
       </c>
       <c r="G53" t="inlineStr"/>
@@ -3180,7 +3180,7 @@
         <v>0.3333333333333333</v>
       </c>
       <c r="S53" t="n">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="54">
@@ -3201,7 +3201,7 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>['authorised catch', 'monitoring report']</t>
+          <t>['common fisheries policy', 'conservation of fish stocks', 'sustainable fisheries', 'fishery management', 'environmental indicator', 'fishing regulations', 'data collection', 'environmental monitoring', 'fishing statistics', 'marine environment']</t>
         </is>
       </c>
       <c r="G54" t="inlineStr"/>
@@ -3254,7 +3254,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>['reduction of gas emissions', 'Paris Agreement on Climate Change', 'energy transition', 'sustainable finance']</t>
+          <t>['energy transition', 'climate change policy', 'job creation', 'renewable energy', 'energy efficiency', 'reduction of gas emissions', 'sustainable development', 'energy production', 'investment', 'greenhouse gas']</t>
         </is>
       </c>
       <c r="G55" t="inlineStr"/>
@@ -3281,10 +3281,10 @@
       <c r="P55" t="inlineStr"/>
       <c r="Q55" t="inlineStr"/>
       <c r="R55" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S55" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="56">
@@ -3305,7 +3305,7 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>['heatwave', 'adaptation to climate change', 'natural disaster', 'meteorology']</t>
+          <t>['drought', 'heatwave', 'South America', 'climate change', 'global warming', 'atmospheric conditions', 'desertification', 'adaptation to climate change', 'environmental impact', 'bioclimatology']</t>
         </is>
       </c>
       <c r="G56" t="inlineStr"/>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>['impact of information technology', '5G', 'ecodesign']</t>
+          <t>['European Commission', 'environmental indicator', 'sustainable development', 'telecommunications industry', 'telecommunications equipment', 'telecommunications policy', 'environmental research', 'digital technology', 'energy policy', 'code of conduct']</t>
         </is>
       </c>
       <c r="G57" t="inlineStr"/>
@@ -3384,10 +3384,10 @@
       <c r="P57" t="inlineStr"/>
       <c r="Q57" t="inlineStr"/>
       <c r="R57" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="S57" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="58">
@@ -3408,7 +3408,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>['adaptation to climate change', 'carbon neutrality', 'reduction of gas emissions', 'carbon capture and storage', 'bioclimatology']</t>
+          <t>['climate change', 'climate change policy', 'carbon', 'carbon neutrality', 'sustainable forest management', 'forest conservation', 'wood production', 'forestry policy', 'reduction of gas emissions', 'natural resources']</t>
         </is>
       </c>
       <c r="G58" t="inlineStr"/>
@@ -3438,7 +3438,7 @@
         <v>0.1666666666666667</v>
       </c>
       <c r="S58" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="59">
@@ -3459,7 +3459,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>['open data', 'industrial research', 'data sharing', 'data governance']</t>
+          <t>['sustainable development', 'environmental research', 'data sharing', 'information system', 'database', 'fuel cell', 'hydrogen', 'supply chain', 'technological change', 'environmental impact']</t>
         </is>
       </c>
       <c r="G59" t="inlineStr"/>
@@ -3486,10 +3486,10 @@
       <c r="P59" t="inlineStr"/>
       <c r="Q59" t="inlineStr"/>
       <c r="R59" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S59" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="60">
@@ -3510,7 +3510,7 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>['mixed cropping', 'crop rotation', 'heatwave']</t>
+          <t>['crop yield', 'crop production', 'cereals', 'agricultural performance', 'Türkiye', 'agricultural statistics', 'bad weather', 'atmospheric conditions', 'cereal-growing', 'agricultural situation']</t>
         </is>
       </c>
       <c r="G60" t="inlineStr"/>
@@ -3537,10 +3537,10 @@
       <c r="P60" t="inlineStr"/>
       <c r="Q60" t="inlineStr"/>
       <c r="R60" t="n">
-        <v>0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="S60" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="61">
@@ -3561,7 +3561,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>['silo', 'agricultural area with environmental restrictions', 'fallow', 'mixed cropping']</t>
+          <t>['bad weather', 'cereals', 'maize', 'crop production', 'crop yield', 'agricultural performance', 'agricultural production', 'Russia', 'cereal-growing', 'crop losses']</t>
         </is>
       </c>
       <c r="G61" t="inlineStr"/>
@@ -3588,10 +3588,10 @@
       <c r="P61" t="inlineStr"/>
       <c r="Q61" t="inlineStr"/>
       <c r="R61" t="n">
-        <v>0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="S61" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>